<commit_message>
Fixed some minor issues
</commit_message>
<xml_diff>
--- a/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
+++ b/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformCommitmentOrder_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{77E79944-33AA-46E7-8C31-EE203A6BD855}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E16C5E1A-A786-43A9-95A5-FE0B25F2407E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2040" yWindow="-19815" windowWidth="27780" windowHeight="16545" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -3345,7 +3345,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="83">
+  <cellXfs count="84">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3567,6 +3567,9 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="8" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7485,11 +7488,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="A1:Z46"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C2" activePane="bottomRight" state="frozen"/>
+    <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
+      <pane xSplit="2" ySplit="1" topLeftCell="C37" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J24" sqref="J24"/>
+      <selection pane="bottomRight" activeCell="I41" sqref="I41"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -8742,13 +8745,13 @@
       <c r="H28" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="I28" s="82" t="s">
+      <c r="I28" s="83" t="s">
         <v>658</v>
       </c>
-      <c r="J28" s="82" t="s">
+      <c r="J28" s="83" t="s">
         <v>558</v>
       </c>
-      <c r="K28" s="82" t="s">
+      <c r="K28" s="83" t="s">
         <v>657</v>
       </c>
       <c r="L28" s="2">
@@ -8784,13 +8787,13 @@
       <c r="H29" s="2" t="s">
         <v>470</v>
       </c>
-      <c r="I29" s="82" t="s">
+      <c r="I29" s="83" t="s">
         <v>658</v>
       </c>
-      <c r="J29" s="82" t="s">
+      <c r="J29" s="83" t="s">
         <v>558</v>
       </c>
-      <c r="K29" s="82" t="s">
+      <c r="K29" s="83" t="s">
         <v>657</v>
       </c>
       <c r="L29" s="2">

</xml_diff>

<commit_message>
Added subset and instance
</commit_message>
<xml_diff>
--- a/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
+++ b/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformCommitmentOrder_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7F0723B6-B16A-40A8-9091-7698DA6EA7DE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F21CD0-9262-485F-AC88-D40F3A0BF03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="10718" yWindow="0" windowWidth="10965" windowHeight="13763" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-4065" yWindow="-21600" windowWidth="26025" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$46</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$48</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -140,6 +140,7 @@
     <definedName name="Type_Target_Style">Type!$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
+  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -160,7 +161,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1183" uniqueCount="743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="748">
   <si>
     <t>Definition</t>
   </si>
@@ -2798,9 +2799,6 @@
     <t>A text value for any sentence that can be consecutive to another case(s). By default, a sentence is concurrent to other court case sentences unless specified by a judge.</t>
   </si>
   <si>
-    <t xml:space="preserve"> j:Sentence/nola-ext:SentenceAugmentation/nola-ext:RelatedSentenceAssociation/nc:ActivityIdentification</t>
-  </si>
-  <si>
     <t>ChargeDispositionDecisionText</t>
   </si>
   <si>
@@ -2855,9 +2853,6 @@
     <t>A description of the sentence being imposed.</t>
   </si>
   <si>
-    <t xml:space="preserve"> j:Sentence/nola-ext:SentenceAugmentation/nola-ext:SentenceSpecialCondition</t>
-  </si>
-  <si>
     <t>nola-ext:SentenceAugmentationType</t>
   </si>
   <si>
@@ -2945,9 +2940,6 @@
     <t>12-17-0304</t>
   </si>
   <si>
-    <t>Jhon Doe</t>
-  </si>
-  <si>
     <t>BLACK</t>
   </si>
   <si>
@@ -3029,9 +3021,6 @@
     <t>102 Main St., New Orleans, LA 70032</t>
   </si>
   <si>
-    <t>Jim Smith</t>
-  </si>
-  <si>
     <t>103 Main St., New Orleans, LA 70032</t>
   </si>
   <si>
@@ -3041,9 +3030,6 @@
     <t>j:CourtOrder/nola-ext:CourtOrderAugmentation/nc:Case/j:CaseAugmentation/j:CaseCourt/nola-ext:CourtAugmentation/nc:AddressCountyName</t>
   </si>
   <si>
-    <t xml:space="preserve"> j:Sentence/nola-ext:SentenceAugmentation/nola-ext:RelatedSentenceAssociation/nola-ext:SentenceAssociationCode</t>
-  </si>
-  <si>
     <t>j:Sentence/j:SentenceCharge/nola-ext:ChargeAugmentation/nola-ext:OffenseDate/nc:Date</t>
   </si>
   <si>
@@ -3093,6 +3079,36 @@
   </si>
   <si>
     <t>j:Sentence/j:SentenceCharge/j:ChargeEnhancingAllegationCharge</t>
+  </si>
+  <si>
+    <t>j:Sentence/nola-ext:SentenceAugmentation/nola-ext:RelatedSentenceAssociation/nc:ActivityIdentification</t>
+  </si>
+  <si>
+    <t>j:Sentence/nola-ext:SentenceAugmentation/nola-ext:RelatedSentenceAssociation/nola-ext:SentenceAssociationCode</t>
+  </si>
+  <si>
+    <t>j:Sentence/nola-ext:SentenceAugmentation/nola-ext:SentenceSpecialConditionText</t>
+  </si>
+  <si>
+    <t>John Doe</t>
+  </si>
+  <si>
+    <t>Hon. Jim Smith</t>
+  </si>
+  <si>
+    <t>j:Sentence/nola-ext:SentenceAugmentation/ j:Incarceration/ j:SupervisionAugmentation/ j:SupervisionAssignedTerm/j:TermLifeIndicator</t>
+  </si>
+  <si>
+    <t>j:TermLifeIndicator</t>
+  </si>
+  <si>
+    <t>niem-xsd:boolean</t>
+  </si>
+  <si>
+    <t>True if the term is not for a set duration length but for life; false otherwise.</t>
+  </si>
+  <si>
+    <t>j:Sentence/j:SentecenTerm/j:TermLifeIndicator</t>
   </si>
 </sst>
 </file>
@@ -3452,7 +3468,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3685,6 +3701,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -3773,9 +3792,6 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <font>
         <b val="0"/>
         <i val="0"/>
@@ -4592,6 +4608,9 @@
           <bgColor auto="1"/>
         </patternFill>
       </fill>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
+    <dxf>
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
     <dxf>
@@ -4866,43 +4885,43 @@
 </file>
 
 <file path=xl/tables/table10.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="30" dataDxfId="29" tableBorderDxfId="28" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="10" xr:uid="{733D753A-1A77-494A-B62C-0EC743EEA49A}" name="Table10" displayName="Table10" ref="A1:N2" totalsRowShown="0" headerRowDxfId="29" dataDxfId="28" tableBorderDxfId="27" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{E1E5EF99-DFA3-4734-B0F5-3FD6CA399E33}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="27"/>
-    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="26"/>
-    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="25"/>
-    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="24"/>
-    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="23"/>
-    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="22"/>
-    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="21"/>
-    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="20"/>
-    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="19"/>
-    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="18"/>
-    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="17"/>
-    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="16"/>
-    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="15"/>
-    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="14"/>
+    <tableColumn id="1" xr3:uid="{E1238927-B089-4D9E-8088-75D3EC35BFBA}" name="Source_x000a_NS Prefix" dataDxfId="26"/>
+    <tableColumn id="2" xr3:uid="{9410951A-EE35-4F3C-8F36-8BEE201CF8AF}" name="URI" dataDxfId="25"/>
+    <tableColumn id="3" xr3:uid="{2B517D23-941B-4B3E-A7DD-F7786E3924D5}" name="Definition" dataDxfId="24"/>
+    <tableColumn id="4" xr3:uid="{7DD55007-8311-4C82-A5D2-EBEDF474C65D}" name="Mapping_x000a_Code" dataDxfId="23"/>
+    <tableColumn id="5" xr3:uid="{0E949C96-18B4-4EB9-95F2-53DB84718832}" name="Description" dataDxfId="22"/>
+    <tableColumn id="6" xr3:uid="{E124F618-8325-4FF3-8BF4-E24907425ADE}" name="Notes" dataDxfId="21"/>
+    <tableColumn id="7" xr3:uid="{86983FC7-E843-4CB8-B776-1ACA5758C454}" name="Target_x000a_NS Prefix" dataDxfId="20"/>
+    <tableColumn id="8" xr3:uid="{F92DB840-CE8A-4128-8BB8-B8742F926D09}" name="Style" dataDxfId="19"/>
+    <tableColumn id="9" xr3:uid="{9202EAB5-4BBC-4DFA-8B29-56D32F2F95E2}" name="URI " dataDxfId="18"/>
+    <tableColumn id="10" xr3:uid="{BE82DF52-562E-40A7-B97A-C4017DCE324F}" name="Definition " dataDxfId="17"/>
+    <tableColumn id="11" xr3:uid="{834B3B3E-609B-4AA7-A013-2F95C8CA6ED1}" name="NDR Target" dataDxfId="16"/>
+    <tableColumn id="12" xr3:uid="{9C74517B-484A-41A5-B478-1107D7B7563E}" name="File Name" dataDxfId="15"/>
+    <tableColumn id="13" xr3:uid="{00E1E65A-D173-41FF-8A1D-F764DB3C85EB}" name="Relative Path" dataDxfId="14"/>
+    <tableColumn id="14" xr3:uid="{1A319080-CB5B-4F50-8EF6-DA7F3E87061A}" name="Draft Version" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table11.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="13" dataDxfId="12" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="11" xr:uid="{6A256153-0806-4BEE-936A-A12F0A0B7383}" name="Table11" displayName="Table11" ref="A1:K2" totalsRowShown="0" headerRowDxfId="12" dataDxfId="11" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:K2" xr:uid="{79E81683-51FB-4FF9-9289-31DDA054DB7A}"/>
   <tableColumns count="11">
-    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="10"/>
-    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="9"/>
-    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="8"/>
-    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="7"/>
-    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="6"/>
-    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="5"/>
-    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="4"/>
-    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="3"/>
-    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="2"/>
-    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="1"/>
+    <tableColumn id="1" xr3:uid="{B23F336D-16B9-4C95-BE96-F5283EAE0F3C}" name="Source_x000a_NS Prefix" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{0D056408-CA8F-4336-AED7-3818011F9385}" name="Term" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{90A93FC4-10F0-4295-AC5C-E2A951CBA7BC}" name="Literal" dataDxfId="8"/>
+    <tableColumn id="4" xr3:uid="{A1AC1DB1-AA7D-48B2-9765-4E5BA52F23DE}" name="Definition" dataDxfId="7"/>
+    <tableColumn id="5" xr3:uid="{BD7B43BD-647B-4803-8F9F-0147C7FD23A4}" name="Mapping_x000a_Code" dataDxfId="6"/>
+    <tableColumn id="6" xr3:uid="{72609C76-FA3F-40C0-B5FF-60D4974FFD61}" name="Description" dataDxfId="5"/>
+    <tableColumn id="7" xr3:uid="{479204AB-0608-4CE8-8D22-F418523DDDA2}" name="Notes" dataDxfId="4"/>
+    <tableColumn id="8" xr3:uid="{2C9C9513-0007-44E3-8DFD-9FDD58431071}" name="Target_x000a_NS Prefix" dataDxfId="3"/>
+    <tableColumn id="9" xr3:uid="{1442C4F6-90A1-4765-A362-538E7A781367}" name="Term " dataDxfId="2"/>
+    <tableColumn id="10" xr3:uid="{92198433-569D-43D9-9243-453965C7540B}" name="Literal " dataDxfId="1"/>
+    <tableColumn id="11" xr3:uid="{38E45C62-D7D7-487A-BB8B-582528BBD31D}" name="Definition " dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -4950,108 +4969,108 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y46" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Y46" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
-  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y46">
-    <sortCondition ref="O1:O46"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y48" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Y48" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y48">
+    <sortCondition ref="O1:O48"/>
   </sortState>
   <tableColumns count="25">
     <tableColumn id="1" xr3:uid="{00000000-0010-0000-0500-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="104"/>
     <tableColumn id="2" xr3:uid="{00000000-0010-0000-0500-000002000000}" name="Property Name" dataDxfId="103"/>
     <tableColumn id="3" xr3:uid="{00000000-0010-0000-0500-000003000000}" name="Data Type" dataDxfId="102"/>
-    <tableColumn id="18" xr3:uid="{15ED65A4-A152-4480-A2B4-9AA1E45F09B9}" name="Definition" dataDxfId="0"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Example" dataDxfId="101"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="100"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="99"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="98"/>
-    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="97"/>
-    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="96"/>
-    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="95"/>
-    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="94"/>
-    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="93"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="92"/>
-    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="91"/>
-    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="90"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="89"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="88"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="87"/>
-    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="86"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="85"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="84"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="83"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="82"/>
-    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="81"/>
+    <tableColumn id="18" xr3:uid="{15ED65A4-A152-4480-A2B4-9AA1E45F09B9}" name="Definition" dataDxfId="101"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0500-000004000000}" name="Example" dataDxfId="100"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0500-000005000000}" name="Mapping_x000a_Code" dataDxfId="99"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0500-000006000000}" name="Description" dataDxfId="98"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0500-000007000000}" name="Notes" dataDxfId="97"/>
+    <tableColumn id="24" xr3:uid="{B256BE0E-1B95-49D2-BF5B-AD5320663854}" name="EDM Class" dataDxfId="96"/>
+    <tableColumn id="23" xr3:uid="{C5C0958E-E98B-4096-B70E-A6517F49A64D}" name="EDM Attribute" dataDxfId="95"/>
+    <tableColumn id="14" xr3:uid="{70B266EE-E89C-4B0F-ACFB-6BBC1BBE7978}" name="EDM Type" dataDxfId="94"/>
+    <tableColumn id="26" xr3:uid="{B613C991-CC70-4831-83C3-97449E0A59FB}" name="EDM Definition" dataDxfId="93"/>
+    <tableColumn id="27" xr3:uid="{9FF11716-702A-419A-91F2-858D4D3B16EE}" name="EDM Cardinality" dataDxfId="92"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0500-000008000000}" name="Target_x000a_NS Prefix" dataDxfId="91"/>
+    <tableColumn id="20" xr3:uid="{8CFFA3EE-5D28-4D5E-86E0-9F9851A3E676}" name="NIEM XPath" dataDxfId="90"/>
+    <tableColumn id="25" xr3:uid="{161AA4D8-B799-4722-BAB9-DA7BA3B360DA}" name="NIEM Type" dataDxfId="89"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0500-000009000000}" name="NIEM Property Name " dataDxfId="88"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0500-00000A000000}" name="NIEM Qualified Data Type" dataDxfId="87"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0500-00000B000000}" name="NIEM Definition " dataDxfId="86"/>
+    <tableColumn id="19" xr3:uid="{C2DBDA77-E9BC-497B-A1D8-611484B019B5}" name="Cardinality2" dataDxfId="85"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0500-00000C000000}" name="NIEM Qualified Substitution Group" dataDxfId="84"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0500-00000D000000}" name="Style_x000a_default=element" dataDxfId="83"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0500-00000F000000}" name="Keywords" dataDxfId="82"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0500-000010000000}" name="Example Content" dataDxfId="81"/>
+    <tableColumn id="17" xr3:uid="{00000000-0010-0000-0500-000011000000}" name="Usage Info" dataDxfId="80"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table7.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="80" dataDxfId="79" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="7" xr:uid="{8578AF98-37D1-469F-9DF8-407CA14E272E}" name="Table7" displayName="Table7" ref="A1:N2" insertRow="1" totalsRowShown="0" headerRowDxfId="79" dataDxfId="78" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:N2" xr:uid="{C7C77A82-0E27-43B2-B802-78C571058434}"/>
   <tableColumns count="14">
-    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="78"/>
-    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="77"/>
-    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="76"/>
-    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="75"/>
-    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="74"/>
-    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="73"/>
-    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="72"/>
-    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="71"/>
-    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="70"/>
-    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="69"/>
-    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="68"/>
-    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="67"/>
-    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="66"/>
-    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="65"/>
+    <tableColumn id="1" xr3:uid="{2DA18095-6134-4F51-B45C-1FD29868E9D3}" name="Source_x000a_NS Prefix" dataDxfId="77"/>
+    <tableColumn id="2" xr3:uid="{BB7222D3-DF23-4FB4-AACC-7074C8351301}" name="Type Name" dataDxfId="76"/>
+    <tableColumn id="3" xr3:uid="{3AFA1B4A-1B7D-4408-95C4-5D276F6AFCE8}" name="Parent / Base Type" dataDxfId="75"/>
+    <tableColumn id="4" xr3:uid="{DA420D7E-BF45-4DFA-A327-6F5816081658}" name="Definition" dataDxfId="74"/>
+    <tableColumn id="5" xr3:uid="{F0EC8E3B-3924-4431-8523-4FE53C5BC2F9}" name="Mapping_x000a_Code" dataDxfId="73"/>
+    <tableColumn id="6" xr3:uid="{529DD89A-D9F2-4643-B653-535C5D5260B2}" name="Description" dataDxfId="72"/>
+    <tableColumn id="7" xr3:uid="{6A865D88-3AC4-4546-981B-9A5A7EB8F351}" name="Notes" dataDxfId="71"/>
+    <tableColumn id="8" xr3:uid="{FF25761D-56AD-4BA0-8910-6C18CBA6D0CD}" name="Target_x000a_NS Prefix" dataDxfId="70"/>
+    <tableColumn id="9" xr3:uid="{B5902010-EF7D-4FA2-B2B6-B491046CA96D}" name="Type Name " dataDxfId="69"/>
+    <tableColumn id="10" xr3:uid="{422CF2D7-F9C5-4193-9DD3-943BF799ABB8}" name="Qualified Parent / Base Type " dataDxfId="68"/>
+    <tableColumn id="11" xr3:uid="{E69F557F-28BC-41CA-B77C-8F0F1781F3F8}" name="Definition " dataDxfId="67"/>
+    <tableColumn id="12" xr3:uid="{33FAD9D1-2E3A-4DD0-99A3-80B7DC1320DF}" name="Style _x000a_default=object" dataDxfId="66"/>
+    <tableColumn id="13" xr3:uid="{A3613263-4395-41B2-9149-1319C9DE1572}" name="Qualified Union Member Types_x000a_comma-separated list" dataDxfId="65"/>
+    <tableColumn id="14" xr3:uid="{DA9EC388-28FD-4FFC-9EB0-04AF1B5F2EBE}" name="Qualified Metadata Applies to Types_x000a_comma-separated list" dataDxfId="64"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table8.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="64" dataDxfId="63">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="8" xr:uid="{00000000-000C-0000-FFFF-FFFF06000000}" name="Table8" displayName="Table8" ref="A1:Q2" insertRow="1" totalsRowShown="0" headerRowDxfId="63" dataDxfId="62">
   <autoFilter ref="A1:Q2" xr:uid="{00000000-0009-0000-0100-000008000000}"/>
   <tableColumns count="17">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="62"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="61"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="60"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="59"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="58"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="57"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="56"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="55"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="54"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="53"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="52"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="51"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="50"/>
-    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="49"/>
-    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="48"/>
-    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="47"/>
-    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="46"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0600-000001000000}" name="Source_x000a_Type NS" dataDxfId="61"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0600-000002000000}" name="Type Name" dataDxfId="60"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0600-000003000000}" name="Property NS" dataDxfId="59"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0600-000004000000}" name="Property Name" dataDxfId="58"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0600-000005000000}" name="Min" dataDxfId="57"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0600-000006000000}" name="Max" dataDxfId="56"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0600-000007000000}" name="Mapping_x000a_Code" dataDxfId="55"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0600-000008000000}" name="Description" dataDxfId="54"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0600-000009000000}" name="Notes" dataDxfId="53"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0600-00000A000000}" name="Target_x000a_Type NS" dataDxfId="52"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0600-00000B000000}" name="Type Name " dataDxfId="51"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0600-00000C000000}" name="Property NS " dataDxfId="50"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0600-00000D000000}" name="Property Name " dataDxfId="49"/>
+    <tableColumn id="14" xr3:uid="{00000000-0010-0000-0600-00000E000000}" name="Min_x000a_(default=0)" dataDxfId="48"/>
+    <tableColumn id="15" xr3:uid="{00000000-0010-0000-0600-00000F000000}" name="Max (default_x000a_=unbounded)" dataDxfId="47"/>
+    <tableColumn id="16" xr3:uid="{00000000-0010-0000-0600-000010000000}" name="Definition_x000a_For an external property in an adapter type" dataDxfId="46"/>
+    <tableColumn id="17" xr3:uid="{78D268D1-27FA-4E25-9781-8F942EC05BA0}" name="Sequence" dataDxfId="45"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table9.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="45" dataDxfId="44" headerRowCellStyle="Accent2">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="13" xr:uid="{00000000-000C-0000-FFFF-FFFF07000000}" name="Table13" displayName="Table13" ref="A1:M2" totalsRowShown="0" headerRowDxfId="44" dataDxfId="43" headerRowCellStyle="Accent2">
   <autoFilter ref="A1:M2" xr:uid="{00000000-0009-0000-0100-00000D000000}"/>
   <tableColumns count="13">
-    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="43"/>
-    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="42"/>
-    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="41"/>
-    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="40"/>
-    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="39"/>
-    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="38"/>
-    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="37"/>
-    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="36"/>
-    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="35"/>
-    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="34"/>
-    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="33"/>
-    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="32"/>
-    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="31"/>
+    <tableColumn id="1" xr3:uid="{00000000-0010-0000-0700-000001000000}" name="Source_x000a_NS Prefix" dataDxfId="42"/>
+    <tableColumn id="2" xr3:uid="{00000000-0010-0000-0700-000002000000}" name="Type Name" dataDxfId="41"/>
+    <tableColumn id="3" xr3:uid="{00000000-0010-0000-0700-000003000000}" name="Value" dataDxfId="40"/>
+    <tableColumn id="4" xr3:uid="{00000000-0010-0000-0700-000004000000}" name="Definition" dataDxfId="39"/>
+    <tableColumn id="5" xr3:uid="{00000000-0010-0000-0700-000005000000}" name="Style_x000a_default=enumeration" dataDxfId="38"/>
+    <tableColumn id="6" xr3:uid="{00000000-0010-0000-0700-000006000000}" name="Mapping_x000a_Code" dataDxfId="37"/>
+    <tableColumn id="7" xr3:uid="{00000000-0010-0000-0700-000007000000}" name="Description" dataDxfId="36"/>
+    <tableColumn id="8" xr3:uid="{00000000-0010-0000-0700-000008000000}" name="Notes" dataDxfId="35"/>
+    <tableColumn id="9" xr3:uid="{00000000-0010-0000-0700-000009000000}" name="Target_x000a_NS Prefix" dataDxfId="34"/>
+    <tableColumn id="10" xr3:uid="{00000000-0010-0000-0700-00000A000000}" name="Type Name " dataDxfId="33"/>
+    <tableColumn id="11" xr3:uid="{00000000-0010-0000-0700-00000B000000}" name="Value " dataDxfId="32"/>
+    <tableColumn id="12" xr3:uid="{00000000-0010-0000-0700-00000C000000}" name="Definition " dataDxfId="31"/>
+    <tableColumn id="13" xr3:uid="{00000000-0010-0000-0700-00000D000000}" name="Style_x000a_default=enumeration " dataDxfId="30"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight8" showFirstColumn="0" showLastColumn="0" showRowStripes="0" showColumnStripes="0"/>
 </table>
@@ -7606,13 +7625,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA46"/>
+  <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="K44" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="J46" sqref="J46"/>
+      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7656,7 +7675,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>689</v>
+        <v>687</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>49</v>
@@ -7722,2077 +7741,2185 @@
         <v>625</v>
       </c>
     </row>
-    <row r="2" spans="1:27" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="2" spans="1:27" ht="185.25" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
-        <v>387</v>
+        <v>379</v>
       </c>
       <c r="C2" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D2" s="2" t="s">
-        <v>431</v>
-      </c>
-      <c r="E2" s="85" t="s">
-        <v>703</v>
+        <v>396</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>694</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>639</v>
+        <v>596</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>550</v>
+        <v>572</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>638</v>
+        <v>597</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
       <c r="O2" s="82" t="s">
-        <v>644</v>
+        <v>722</v>
       </c>
       <c r="P2" s="82" t="s">
-        <v>640</v>
+        <v>599</v>
       </c>
       <c r="Q2" s="82" t="s">
-        <v>518</v>
+        <v>601</v>
       </c>
       <c r="R2" s="82" t="s">
-        <v>489</v>
-      </c>
-      <c r="S2" s="82" t="s">
-        <v>642</v>
+        <v>481</v>
+      </c>
+      <c r="S2" s="2" t="s">
+        <v>602</v>
       </c>
       <c r="U2" s="2"/>
       <c r="AA2" s="82" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="3" spans="1:27" ht="285" x14ac:dyDescent="0.45">
+    <row r="3" spans="1:27" ht="185.25" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
-        <v>388</v>
+        <v>379</v>
       </c>
       <c r="C3" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D3" s="2" t="s">
-        <v>407</v>
-      </c>
-      <c r="E3" s="85" t="s">
-        <v>704</v>
+        <v>396</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>694</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>470</v>
+        <v>530</v>
       </c>
       <c r="J3" s="2" t="s">
-        <v>639</v>
+        <v>467</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>550</v>
+        <v>572</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>638</v>
+        <v>531</v>
       </c>
       <c r="M3" s="2">
         <v>1</v>
       </c>
+      <c r="N3" s="82"/>
       <c r="O3" s="82" t="s">
-        <v>644</v>
+        <v>723</v>
       </c>
       <c r="P3" s="82" t="s">
-        <v>640</v>
+        <v>600</v>
       </c>
       <c r="Q3" s="82" t="s">
-        <v>518</v>
+        <v>604</v>
       </c>
       <c r="R3" s="82" t="s">
-        <v>489</v>
-      </c>
-      <c r="S3" s="82" t="s">
-        <v>642</v>
+        <v>598</v>
+      </c>
+      <c r="S3" s="2" t="s">
+        <v>603</v>
       </c>
       <c r="U3" s="2"/>
       <c r="AA3" s="82" t="s">
         <v>589</v>
       </c>
     </row>
-    <row r="4" spans="1:27" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="4" spans="1:27" ht="313.5" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
-        <v>360</v>
+        <v>381</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>359</v>
+        <v>424</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>462</v>
+        <v>398</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>701</v>
+        <v>712</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>548</v>
+        <v>536</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>469</v>
+        <v>534</v>
       </c>
       <c r="K4" s="2" t="s">
         <v>550</v>
       </c>
       <c r="L4" s="2" t="s">
-        <v>643</v>
+        <v>537</v>
       </c>
       <c r="M4" s="2" t="s">
         <v>533</v>
       </c>
-      <c r="O4" s="82" t="s">
-        <v>644</v>
-      </c>
-      <c r="P4" s="82" t="s">
-        <v>640</v>
-      </c>
-      <c r="Q4" s="82" t="s">
-        <v>518</v>
-      </c>
-      <c r="R4" s="82" t="s">
-        <v>489</v>
-      </c>
-      <c r="S4" s="82" t="s">
-        <v>642</v>
+      <c r="O4" s="2" t="s">
+        <v>541</v>
+      </c>
+      <c r="P4" s="2" t="s">
+        <v>542</v>
+      </c>
+      <c r="Q4" s="2" t="s">
+        <v>539</v>
+      </c>
+      <c r="R4" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="S4" s="2" t="s">
+        <v>537</v>
       </c>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="399" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" ht="313.5" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
-        <v>386</v>
+        <v>381</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>359</v>
+        <v>424</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>406</v>
+        <v>398</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>702</v>
+        <v>713</v>
       </c>
       <c r="I5" s="2" t="s">
-        <v>470</v>
+        <v>536</v>
       </c>
       <c r="J5" s="2" t="s">
-        <v>637</v>
+        <v>535</v>
       </c>
       <c r="K5" s="2" t="s">
-        <v>572</v>
+        <v>550</v>
       </c>
       <c r="L5" s="2" t="s">
-        <v>636</v>
-      </c>
-      <c r="M5" s="2">
-        <v>1</v>
+        <v>538</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>533</v>
       </c>
       <c r="O5" s="82" t="s">
         <v>725</v>
       </c>
       <c r="P5" s="82" t="s">
-        <v>641</v>
+        <v>726</v>
       </c>
       <c r="Q5" s="82" t="s">
-        <v>635</v>
+        <v>727</v>
       </c>
       <c r="R5" s="82" t="s">
         <v>481</v>
       </c>
-      <c r="S5" s="82" t="s">
-        <v>636</v>
+      <c r="S5" s="2" t="s">
+        <v>540</v>
       </c>
       <c r="U5" s="2"/>
     </row>
-    <row r="6" spans="1:27" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="6" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B6" s="2" t="s">
-        <v>365</v>
+        <v>443</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>424</v>
+        <v>357</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>464</v>
+        <v>438</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>708</v>
+        <v>691</v>
       </c>
       <c r="I6" s="2" t="s">
-        <v>460</v>
+        <v>505</v>
       </c>
       <c r="J6" s="2" t="s">
-        <v>460</v>
+        <v>458</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="L6" s="82" t="s">
-        <v>464</v>
+        <v>569</v>
+      </c>
+      <c r="L6" s="2" t="s">
+        <v>506</v>
       </c>
       <c r="M6" s="2" t="s">
-        <v>533</v>
+        <v>479</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>663</v>
+        <v>507</v>
       </c>
       <c r="P6" s="2" t="s">
-        <v>664</v>
+        <v>495</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>665</v>
+        <v>508</v>
       </c>
       <c r="R6" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="S6" s="82" t="s">
-        <v>464</v>
+      <c r="S6" s="2" t="s">
+        <v>506</v>
       </c>
       <c r="U6" s="2"/>
       <c r="AA6" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="7" spans="1:27" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="7" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B7" s="2" t="s">
-        <v>383</v>
+        <v>444</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>220</v>
+        <v>358</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>402</v>
-      </c>
-      <c r="E7" s="85" t="s">
-        <v>698</v>
+        <v>437</v>
+      </c>
+      <c r="E7" s="2" t="s">
+        <v>692</v>
       </c>
       <c r="I7" s="2" t="s">
-        <v>552</v>
+        <v>505</v>
       </c>
       <c r="J7" s="2" t="s">
-        <v>554</v>
+        <v>459</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>555</v>
+        <v>570</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>556</v>
+        <v>510</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O7" s="82" t="s">
-        <v>726</v>
-      </c>
-      <c r="P7" s="82" t="s">
-        <v>626</v>
+      <c r="O7" s="2" t="s">
+        <v>511</v>
+      </c>
+      <c r="P7" s="2" t="s">
+        <v>495</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>514</v>
+        <v>509</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>515</v>
-      </c>
-      <c r="S7" s="82" t="s">
-        <v>556</v>
+        <v>481</v>
+      </c>
+      <c r="S7" s="2" t="s">
+        <v>510</v>
       </c>
       <c r="U7" s="2"/>
       <c r="AA7" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="8" spans="1:27" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="8" spans="1:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
-        <v>379</v>
+        <v>445</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>424</v>
+        <v>220</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>396</v>
-      </c>
-      <c r="E8" s="2" t="s">
-        <v>697</v>
+        <v>393</v>
+      </c>
+      <c r="E8" s="83" t="s">
+        <v>693</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>530</v>
+        <v>512</v>
       </c>
       <c r="J8" s="2" t="s">
-        <v>596</v>
+        <v>455</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>597</v>
-      </c>
-      <c r="M8" s="2">
-        <v>1</v>
-      </c>
-      <c r="O8" s="82" t="s">
-        <v>727</v>
-      </c>
-      <c r="P8" s="82" t="s">
-        <v>599</v>
-      </c>
-      <c r="Q8" s="82" t="s">
-        <v>601</v>
-      </c>
-      <c r="R8" s="82" t="s">
-        <v>481</v>
+        <v>513</v>
+      </c>
+      <c r="M8" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="O8" s="2" t="s">
+        <v>516</v>
+      </c>
+      <c r="P8" s="2" t="s">
+        <v>582</v>
+      </c>
+      <c r="Q8" s="2" t="s">
+        <v>514</v>
+      </c>
+      <c r="R8" s="2" t="s">
+        <v>515</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>602</v>
+        <v>513</v>
       </c>
       <c r="U8" s="2"/>
       <c r="AA8" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="9" spans="1:27" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="9" spans="1:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B9" s="2" t="s">
-        <v>379</v>
+        <v>441</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>424</v>
+        <v>433</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>396</v>
+        <v>435</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>697</v>
+        <v>709</v>
       </c>
       <c r="I9" s="2" t="s">
-        <v>530</v>
+        <v>492</v>
       </c>
       <c r="J9" s="2" t="s">
-        <v>467</v>
+        <v>457</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>572</v>
+        <v>566</v>
       </c>
       <c r="L9" s="2" t="s">
-        <v>531</v>
-      </c>
-      <c r="M9" s="2">
-        <v>1</v>
-      </c>
-      <c r="N9" s="82"/>
-      <c r="O9" s="82" t="s">
-        <v>728</v>
-      </c>
-      <c r="P9" s="82" t="s">
-        <v>600</v>
-      </c>
-      <c r="Q9" s="82" t="s">
-        <v>604</v>
-      </c>
-      <c r="R9" s="82" t="s">
-        <v>598</v>
+        <v>491</v>
+      </c>
+      <c r="M9" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="O9" s="2" t="s">
+        <v>493</v>
+      </c>
+      <c r="P9" s="2" t="s">
+        <v>583</v>
+      </c>
+      <c r="Q9" s="2" t="s">
+        <v>498</v>
+      </c>
+      <c r="R9" s="2" t="s">
+        <v>481</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>603</v>
+        <v>584</v>
       </c>
       <c r="U9" s="2"/>
       <c r="AA9" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="10" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="10" spans="1:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B10" s="2" t="s">
-        <v>384</v>
+        <v>442</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>220</v>
+        <v>434</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>403</v>
-      </c>
-      <c r="E10" s="85" t="s">
-        <v>699</v>
+        <v>439</v>
+      </c>
+      <c r="E10" s="2" t="s">
+        <v>710</v>
       </c>
       <c r="I10" s="2" t="s">
-        <v>679</v>
+        <v>492</v>
       </c>
       <c r="J10" s="2" t="s">
-        <v>680</v>
+        <v>454</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>555</v>
+        <v>567</v>
       </c>
       <c r="L10" s="2" t="s">
-        <v>681</v>
+        <v>500</v>
       </c>
       <c r="M10" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O10" s="2" t="s">
-        <v>729</v>
+        <v>501</v>
       </c>
       <c r="P10" s="2" t="s">
-        <v>628</v>
+        <v>503</v>
       </c>
       <c r="Q10" s="2" t="s">
-        <v>514</v>
+        <v>502</v>
       </c>
       <c r="R10" s="2" t="s">
-        <v>515</v>
+        <v>504</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>629</v>
+        <v>579</v>
       </c>
       <c r="U10" s="2"/>
       <c r="AA10" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="11" spans="1:27" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="11" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B11" s="2" t="s">
-        <v>381</v>
+        <v>440</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>398</v>
+        <v>436</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>715</v>
+        <v>741</v>
       </c>
       <c r="I11" s="2" t="s">
-        <v>536</v>
+        <v>476</v>
       </c>
       <c r="J11" s="2" t="s">
-        <v>534</v>
+        <v>452</v>
       </c>
       <c r="K11" s="2" t="s">
-        <v>550</v>
+        <v>452</v>
       </c>
       <c r="L11" s="2" t="s">
-        <v>537</v>
+        <v>499</v>
       </c>
       <c r="M11" s="2" t="s">
-        <v>533</v>
+        <v>479</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>541</v>
+        <v>728</v>
       </c>
       <c r="P11" s="2" t="s">
-        <v>542</v>
+        <v>494</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>539</v>
+        <v>665</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>481</v>
+        <v>666</v>
       </c>
       <c r="S11" s="2" t="s">
-        <v>537</v>
+        <v>499</v>
       </c>
       <c r="U11" s="2"/>
       <c r="AA11" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="12" spans="1:27" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="12" spans="1:27" ht="171" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
-        <v>381</v>
+        <v>446</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>424</v>
+        <v>427</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>398</v>
-      </c>
-      <c r="E12" s="2" t="s">
-        <v>716</v>
+        <v>447</v>
+      </c>
+      <c r="E12" s="2">
+        <v>999999999</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>536</v>
+        <v>512</v>
       </c>
       <c r="J12" s="2" t="s">
-        <v>535</v>
+        <v>456</v>
       </c>
       <c r="K12" s="2" t="s">
         <v>550</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>538</v>
+        <v>517</v>
       </c>
       <c r="M12" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="O12" s="82" t="s">
-        <v>730</v>
-      </c>
-      <c r="P12" s="82" t="s">
-        <v>731</v>
-      </c>
-      <c r="Q12" s="82" t="s">
-        <v>732</v>
-      </c>
-      <c r="R12" s="82" t="s">
-        <v>481</v>
+        <v>479</v>
+      </c>
+      <c r="O12" s="2" t="s">
+        <v>519</v>
+      </c>
+      <c r="P12" s="2" t="s">
+        <v>581</v>
+      </c>
+      <c r="Q12" s="2" t="s">
+        <v>518</v>
+      </c>
+      <c r="R12" s="2" t="s">
+        <v>489</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>540</v>
+        <v>580</v>
       </c>
       <c r="U12" s="2"/>
       <c r="AA12" s="82" t="s">
         <v>590</v>
       </c>
     </row>
-    <row r="13" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="13" spans="1:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
-        <v>443</v>
+        <v>390</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>357</v>
+        <v>220</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>438</v>
-      </c>
-      <c r="E13" s="2" t="s">
-        <v>694</v>
+        <v>419</v>
+      </c>
+      <c r="E13" s="85" t="s">
+        <v>696</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>505</v>
+        <v>520</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>458</v>
+        <v>521</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>569</v>
+        <v>555</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>506</v>
+        <v>557</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>507</v>
+        <v>729</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>495</v>
+        <v>627</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>508</v>
+        <v>558</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>481</v>
+        <v>559</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>506</v>
+        <v>557</v>
       </c>
       <c r="U13" s="2"/>
       <c r="AA13" s="82" t="s">
         <v>592</v>
       </c>
     </row>
-    <row r="14" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
+    <row r="14" spans="1:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B14" s="2" t="s">
-        <v>444</v>
+        <v>392</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>358</v>
+        <v>423</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>437</v>
+        <v>421</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>695</v>
+        <v>718</v>
       </c>
       <c r="I14" s="2" t="s">
-        <v>505</v>
+        <v>492</v>
       </c>
       <c r="J14" s="2" t="s">
-        <v>459</v>
+        <v>457</v>
       </c>
       <c r="K14" s="2" t="s">
-        <v>570</v>
+        <v>457</v>
       </c>
       <c r="L14" s="2" t="s">
-        <v>510</v>
+        <v>491</v>
       </c>
       <c r="M14" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>511</v>
+        <v>670</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>495</v>
+        <v>583</v>
       </c>
       <c r="Q14" s="2" t="s">
-        <v>509</v>
+        <v>498</v>
       </c>
       <c r="R14" s="2" t="s">
         <v>481</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>510</v>
+        <v>584</v>
       </c>
       <c r="U14" s="2"/>
       <c r="AA14" s="82" t="s">
         <v>593</v>
       </c>
     </row>
-    <row r="15" spans="1:27" ht="114" x14ac:dyDescent="0.45">
+    <row r="15" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B15" s="2" t="s">
-        <v>445</v>
+        <v>391</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>220</v>
+        <v>422</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>393</v>
-      </c>
-      <c r="E15" s="83" t="s">
-        <v>696</v>
+        <v>420</v>
+      </c>
+      <c r="E15" s="2" t="s">
+        <v>742</v>
       </c>
       <c r="I15" s="2" t="s">
-        <v>512</v>
+        <v>476</v>
       </c>
       <c r="J15" s="2" t="s">
-        <v>455</v>
+        <v>452</v>
       </c>
       <c r="K15" s="2" t="s">
-        <v>568</v>
+        <v>452</v>
       </c>
       <c r="L15" s="2" t="s">
-        <v>513</v>
-      </c>
-      <c r="M15" s="2" t="s">
-        <v>479</v>
+        <v>499</v>
+      </c>
+      <c r="M15" s="2">
+        <v>1</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>516</v>
+        <v>730</v>
       </c>
       <c r="P15" s="2" t="s">
-        <v>582</v>
+        <v>494</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>514</v>
+        <v>665</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>515</v>
+        <v>666</v>
       </c>
       <c r="S15" s="2" t="s">
-        <v>513</v>
+        <v>499</v>
       </c>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="114" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" ht="171" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
-        <v>441</v>
+        <v>374</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>433</v>
+        <v>424</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>435</v>
-      </c>
-      <c r="E16" s="2" t="s">
-        <v>712</v>
+        <v>428</v>
+      </c>
+      <c r="E16" s="2">
+        <v>5</v>
       </c>
       <c r="I16" s="2" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="J16" s="2" t="s">
-        <v>457</v>
+        <v>450</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>566</v>
+        <v>550</v>
       </c>
       <c r="L16" s="2" t="s">
-        <v>491</v>
+        <v>480</v>
       </c>
       <c r="M16" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O16" s="2" t="s">
-        <v>493</v>
+      <c r="O16" s="82" t="s">
+        <v>719</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>583</v>
+        <v>585</v>
       </c>
       <c r="Q16" s="2" t="s">
-        <v>498</v>
+        <v>482</v>
       </c>
       <c r="R16" s="2" t="s">
         <v>481</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>584</v>
+        <v>577</v>
       </c>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:27" ht="142.5" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
-        <v>442</v>
+        <v>373</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>434</v>
+        <v>427</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>439</v>
+        <v>448</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>713</v>
+        <v>688</v>
       </c>
       <c r="I17" s="2" t="s">
-        <v>492</v>
+        <v>475</v>
       </c>
       <c r="J17" s="2" t="s">
-        <v>454</v>
+        <v>474</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>567</v>
+        <v>565</v>
       </c>
       <c r="L17" s="2" t="s">
-        <v>500</v>
+        <v>478</v>
       </c>
       <c r="M17" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O17" s="2" t="s">
-        <v>501</v>
+      <c r="O17" s="82" t="s">
+        <v>731</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>503</v>
+        <v>585</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>502</v>
+        <v>732</v>
       </c>
       <c r="R17" s="2" t="s">
-        <v>504</v>
+        <v>481</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>579</v>
+        <v>576</v>
       </c>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:27" ht="185.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
-        <v>440</v>
+        <v>375</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>436</v>
+        <v>429</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="I18" s="2" t="s">
-        <v>476</v>
+        <v>475</v>
       </c>
       <c r="J18" s="2" t="s">
-        <v>452</v>
+        <v>449</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>452</v>
+        <v>550</v>
       </c>
       <c r="L18" s="2" t="s">
-        <v>499</v>
+        <v>483</v>
       </c>
       <c r="M18" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>733</v>
+        <v>720</v>
       </c>
       <c r="P18" s="2" t="s">
-        <v>494</v>
+        <v>497</v>
       </c>
       <c r="Q18" s="2" t="s">
-        <v>667</v>
+        <v>484</v>
       </c>
       <c r="R18" s="2" t="s">
-        <v>668</v>
+        <v>481</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>499</v>
+        <v>575</v>
       </c>
       <c r="U18" s="2"/>
       <c r="AA18" s="82" t="s">
         <v>594</v>
       </c>
     </row>
-    <row r="19" spans="2:27" ht="171" x14ac:dyDescent="0.45">
+    <row r="19" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B19" s="2" t="s">
-        <v>446</v>
+        <v>384</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>427</v>
+        <v>220</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>447</v>
-      </c>
-      <c r="E19" s="2">
-        <v>999999999</v>
+        <v>403</v>
+      </c>
+      <c r="E19" s="85" t="s">
+        <v>696</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>512</v>
+        <v>677</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>456</v>
+        <v>678</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>550</v>
+        <v>555</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>517</v>
+        <v>679</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>519</v>
+        <v>724</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>581</v>
+        <v>628</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>489</v>
+        <v>515</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>580</v>
+        <v>629</v>
       </c>
       <c r="U19" s="2"/>
     </row>
-    <row r="20" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+    <row r="20" spans="2:27" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B20" s="2" t="s">
-        <v>390</v>
+        <v>371</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>220</v>
+        <v>423</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>419</v>
-      </c>
-      <c r="E20" s="85" t="s">
-        <v>699</v>
+        <v>418</v>
+      </c>
+      <c r="E20" s="2" t="s">
+        <v>717</v>
       </c>
       <c r="I20" s="2" t="s">
-        <v>520</v>
+        <v>492</v>
       </c>
       <c r="J20" s="2" t="s">
-        <v>521</v>
+        <v>457</v>
       </c>
       <c r="K20" s="2" t="s">
-        <v>555</v>
+        <v>457</v>
       </c>
       <c r="L20" s="2" t="s">
-        <v>557</v>
+        <v>491</v>
       </c>
       <c r="M20" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>734</v>
+        <v>674</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>627</v>
+        <v>583</v>
       </c>
       <c r="Q20" s="2" t="s">
-        <v>558</v>
+        <v>498</v>
       </c>
       <c r="R20" s="2" t="s">
-        <v>559</v>
+        <v>481</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>557</v>
+        <v>584</v>
       </c>
       <c r="U20" s="2"/>
     </row>
     <row r="21" spans="2:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B21" s="2" t="s">
-        <v>392</v>
+        <v>370</v>
       </c>
       <c r="C21" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>416</v>
+      </c>
+      <c r="E21" s="85" t="s">
+        <v>716</v>
+      </c>
+      <c r="I21" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="J21" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="K21" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="L21" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="M21" s="2">
+        <v>1</v>
+      </c>
+      <c r="O21" s="2" t="s">
+        <v>673</v>
+      </c>
+      <c r="P21" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q21" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="R21" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="S21" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="U21" s="2"/>
+    </row>
+    <row r="22" spans="2:27" ht="156.75" x14ac:dyDescent="0.45">
+      <c r="B22" s="2" t="s">
+        <v>368</v>
+      </c>
+      <c r="C22" s="2" t="s">
         <v>423</v>
       </c>
-      <c r="D21" s="2" t="s">
-        <v>421</v>
-      </c>
-      <c r="E21" s="2" t="s">
-        <v>722</v>
-      </c>
-      <c r="I21" s="2" t="s">
+      <c r="D22" s="2" t="s">
+        <v>417</v>
+      </c>
+      <c r="E22" s="2" t="s">
+        <v>708</v>
+      </c>
+      <c r="I22" s="2" t="s">
         <v>492</v>
       </c>
-      <c r="J21" s="2" t="s">
+      <c r="J22" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="K21" s="2" t="s">
+      <c r="K22" s="2" t="s">
         <v>457</v>
       </c>
-      <c r="L21" s="2" t="s">
+      <c r="L22" s="2" t="s">
         <v>491</v>
       </c>
-      <c r="M21" s="2" t="s">
+      <c r="M22" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O21" s="2" t="s">
+      <c r="O22" s="2" t="s">
         <v>672</v>
       </c>
-      <c r="P21" s="2" t="s">
+      <c r="P22" s="2" t="s">
         <v>583</v>
       </c>
-      <c r="Q21" s="2" t="s">
+      <c r="Q22" s="2" t="s">
         <v>498</v>
       </c>
-      <c r="R21" s="2" t="s">
+      <c r="R22" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="S21" s="2" t="s">
+      <c r="S22" s="2" t="s">
         <v>584</v>
-      </c>
-      <c r="U21" s="2"/>
-    </row>
-    <row r="22" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
-      <c r="B22" s="2" t="s">
-        <v>391</v>
-      </c>
-      <c r="C22" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D22" s="2" t="s">
-        <v>420</v>
-      </c>
-      <c r="E22" s="2" t="s">
-        <v>721</v>
-      </c>
-      <c r="I22" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="J22" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="K22" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="L22" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="M22" s="2">
-        <v>1</v>
-      </c>
-      <c r="O22" s="2" t="s">
-        <v>735</v>
-      </c>
-      <c r="P22" s="2" t="s">
-        <v>494</v>
-      </c>
-      <c r="Q22" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="R22" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="S22" s="2" t="s">
-        <v>499</v>
       </c>
       <c r="U22" s="2"/>
       <c r="AA22" s="82" t="s">
         <v>595</v>
       </c>
     </row>
-    <row r="23" spans="2:27" ht="171" x14ac:dyDescent="0.45">
+    <row r="23" spans="2:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B23" s="2" t="s">
-        <v>374</v>
+        <v>367</v>
       </c>
       <c r="C23" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>414</v>
+      </c>
+      <c r="E23" s="85" t="s">
+        <v>707</v>
+      </c>
+      <c r="I23" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="J23" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="K23" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="L23" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="M23" s="2">
+        <v>1</v>
+      </c>
+      <c r="O23" s="2" t="s">
+        <v>671</v>
+      </c>
+      <c r="P23" s="2" t="s">
+        <v>668</v>
+      </c>
+      <c r="Q23" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="R23" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="S23" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="U23" s="2"/>
+    </row>
+    <row r="24" spans="2:27" ht="185.25" x14ac:dyDescent="0.45">
+      <c r="B24" s="2" t="s">
+        <v>376</v>
+      </c>
+      <c r="C24" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D23" s="2" t="s">
-        <v>428</v>
-      </c>
-      <c r="E23" s="2">
-        <v>5</v>
-      </c>
-      <c r="I23" s="2" t="s">
-        <v>475</v>
-      </c>
-      <c r="J23" s="2" t="s">
-        <v>450</v>
-      </c>
-      <c r="K23" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="L23" s="2" t="s">
-        <v>480</v>
-      </c>
-      <c r="M23" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="O23" s="82" t="s">
-        <v>723</v>
-      </c>
-      <c r="P23" s="2" t="s">
-        <v>585</v>
-      </c>
-      <c r="Q23" s="2" t="s">
-        <v>482</v>
-      </c>
-      <c r="R23" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="S23" s="2" t="s">
-        <v>577</v>
-      </c>
-      <c r="U23" s="2"/>
-    </row>
-    <row r="24" spans="2:27" ht="142.5" x14ac:dyDescent="0.45">
-      <c r="B24" s="2" t="s">
-        <v>373</v>
-      </c>
-      <c r="C24" s="2" t="s">
-        <v>427</v>
-      </c>
       <c r="D24" s="2" t="s">
-        <v>448</v>
+        <v>430</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>690</v>
       </c>
       <c r="I24" s="2" t="s">
-        <v>475</v>
+        <v>477</v>
       </c>
       <c r="J24" s="2" t="s">
-        <v>474</v>
+        <v>451</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>565</v>
+        <v>550</v>
       </c>
       <c r="L24" s="2" t="s">
-        <v>478</v>
+        <v>487</v>
       </c>
       <c r="M24" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O24" s="82" t="s">
-        <v>736</v>
+      <c r="O24" s="2" t="s">
+        <v>733</v>
       </c>
       <c r="P24" s="2" t="s">
-        <v>585</v>
+        <v>496</v>
       </c>
       <c r="Q24" s="2" t="s">
-        <v>737</v>
+        <v>490</v>
       </c>
       <c r="R24" s="2" t="s">
-        <v>481</v>
+        <v>489</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>576</v>
+        <v>578</v>
       </c>
       <c r="U24" s="2"/>
       <c r="AA24" s="82" t="s">
         <v>591</v>
       </c>
     </row>
-    <row r="25" spans="2:27" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="25" spans="2:27" ht="114" x14ac:dyDescent="0.45">
       <c r="B25" s="2" t="s">
-        <v>375</v>
+        <v>366</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>424</v>
+        <v>422</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>429</v>
-      </c>
-      <c r="E25" s="2" t="s">
-        <v>691</v>
+        <v>413</v>
+      </c>
+      <c r="E25" s="85" t="s">
+        <v>706</v>
       </c>
       <c r="I25" s="2" t="s">
-        <v>475</v>
+        <v>94</v>
       </c>
       <c r="J25" s="2" t="s">
-        <v>449</v>
+        <v>453</v>
       </c>
       <c r="K25" s="2" t="s">
         <v>550</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>483</v>
+        <v>664</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>724</v>
+        <v>667</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>497</v>
+        <v>668</v>
       </c>
       <c r="Q25" s="2" t="s">
-        <v>484</v>
+        <v>665</v>
       </c>
       <c r="R25" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="S25" s="2" t="s">
+        <v>669</v>
+      </c>
+      <c r="U25" s="2"/>
+    </row>
+    <row r="26" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+      <c r="B26" s="2" t="s">
+        <v>369</v>
+      </c>
+      <c r="C26" s="2" t="s">
+        <v>422</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>415</v>
+      </c>
+      <c r="E26" s="85" t="s">
+        <v>715</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>476</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="K26" s="2" t="s">
+        <v>452</v>
+      </c>
+      <c r="L26" s="2" t="s">
+        <v>499</v>
+      </c>
+      <c r="M26" s="2">
+        <v>1</v>
+      </c>
+      <c r="O26" s="82" t="s">
+        <v>675</v>
+      </c>
+      <c r="P26" s="2" t="s">
+        <v>676</v>
+      </c>
+      <c r="Q26" s="2" t="s">
+        <v>665</v>
+      </c>
+      <c r="R26" s="2" t="s">
+        <v>666</v>
+      </c>
+      <c r="S26" s="82" t="s">
+        <v>685</v>
+      </c>
+      <c r="U26" s="2"/>
+    </row>
+    <row r="27" spans="2:27" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B27" s="2" t="s">
+        <v>409</v>
+      </c>
+      <c r="C27" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>410</v>
+      </c>
+      <c r="E27" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="I27" s="2" t="s">
+        <v>471</v>
+      </c>
+      <c r="J27" s="2" t="s">
+        <v>644</v>
+      </c>
+      <c r="K27" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="L27" s="2" t="s">
+        <v>645</v>
+      </c>
+      <c r="M27" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="O27" s="2" t="s">
+        <v>647</v>
+      </c>
+      <c r="P27" s="2" t="s">
+        <v>574</v>
+      </c>
+      <c r="Q27" s="2" t="s">
+        <v>646</v>
+      </c>
+      <c r="R27" s="2" t="s">
         <v>481</v>
       </c>
-      <c r="S25" s="2" t="s">
-        <v>575</v>
-      </c>
-      <c r="U25" s="2"/>
-    </row>
-    <row r="26" spans="2:27" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="B26" s="2" t="s">
-        <v>371</v>
-      </c>
-      <c r="C26" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="D26" s="2" t="s">
-        <v>418</v>
-      </c>
-      <c r="E26" s="2" t="s">
-        <v>720</v>
-      </c>
-      <c r="I26" s="2" t="s">
-        <v>492</v>
-      </c>
-      <c r="J26" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="K26" s="2" t="s">
-        <v>457</v>
-      </c>
-      <c r="L26" s="2" t="s">
-        <v>491</v>
-      </c>
-      <c r="M26" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="O26" s="2" t="s">
-        <v>676</v>
-      </c>
-      <c r="P26" s="2" t="s">
-        <v>583</v>
-      </c>
-      <c r="Q26" s="2" t="s">
-        <v>498</v>
-      </c>
-      <c r="R26" s="2" t="s">
-        <v>481</v>
-      </c>
-      <c r="S26" s="2" t="s">
-        <v>584</v>
-      </c>
-      <c r="U26" s="2"/>
-    </row>
-    <row r="27" spans="2:27" ht="114" x14ac:dyDescent="0.45">
-      <c r="B27" s="2" t="s">
-        <v>370</v>
-      </c>
-      <c r="C27" s="2" t="s">
-        <v>422</v>
-      </c>
-      <c r="D27" s="2" t="s">
-        <v>416</v>
-      </c>
-      <c r="E27" s="85" t="s">
-        <v>719</v>
-      </c>
-      <c r="I27" s="2" t="s">
-        <v>476</v>
-      </c>
-      <c r="J27" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="K27" s="2" t="s">
-        <v>452</v>
-      </c>
-      <c r="L27" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="M27" s="2">
+      <c r="S27" s="2" t="s">
+        <v>648</v>
+      </c>
+      <c r="U27" s="2"/>
+    </row>
+    <row r="28" spans="2:27" ht="171" x14ac:dyDescent="0.45">
+      <c r="B28" s="2" t="s">
+        <v>378</v>
+      </c>
+      <c r="C28" s="2" t="s">
+        <v>427</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>395</v>
+      </c>
+      <c r="E28" s="2">
         <v>1</v>
       </c>
-      <c r="O27" s="2" t="s">
-        <v>675</v>
-      </c>
-      <c r="P27" s="2" t="s">
-        <v>670</v>
-      </c>
-      <c r="Q27" s="2" t="s">
-        <v>667</v>
-      </c>
-      <c r="R27" s="2" t="s">
-        <v>668</v>
-      </c>
-      <c r="S27" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="U27" s="2"/>
-    </row>
-    <row r="28" spans="2:27" ht="156.75" x14ac:dyDescent="0.45">
-      <c r="B28" s="2" t="s">
-        <v>368</v>
-      </c>
-      <c r="C28" s="2" t="s">
-        <v>423</v>
-      </c>
-      <c r="D28" s="2" t="s">
-        <v>417</v>
-      </c>
-      <c r="E28" s="2" t="s">
-        <v>711</v>
-      </c>
       <c r="I28" s="2" t="s">
-        <v>492</v>
+        <v>525</v>
       </c>
       <c r="J28" s="2" t="s">
-        <v>457</v>
+        <v>466</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>457</v>
+        <v>546</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>491</v>
+        <v>527</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>674</v>
-      </c>
-      <c r="P28" s="2" t="s">
-        <v>583</v>
+        <v>735</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>498</v>
+        <v>528</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>481</v>
+        <v>529</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>584</v>
+        <v>588</v>
       </c>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:27" ht="256.5" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
-        <v>367</v>
+        <v>389</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>422</v>
+        <v>426</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>414</v>
-      </c>
-      <c r="E29" s="85" t="s">
-        <v>710</v>
+        <v>408</v>
+      </c>
+      <c r="E29" s="2">
+        <v>2</v>
       </c>
       <c r="I29" s="2" t="s">
-        <v>476</v>
+        <v>471</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>452</v>
+        <v>523</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>452</v>
+        <v>572</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>499</v>
+        <v>522</v>
       </c>
       <c r="M29" s="2">
         <v>1</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>673</v>
+        <v>734</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>670</v>
+        <v>574</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>667</v>
+        <v>524</v>
       </c>
       <c r="R29" s="2" t="s">
-        <v>668</v>
+        <v>481</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>499</v>
+        <v>573</v>
       </c>
       <c r="U29" s="2"/>
     </row>
-    <row r="30" spans="2:27" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:27" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
-        <v>376</v>
+        <v>380</v>
       </c>
       <c r="C30" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>430</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>692</v>
+        <v>397</v>
+      </c>
+      <c r="E30" s="84">
+        <v>0.6020833333333333</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>477</v>
+        <v>530</v>
       </c>
       <c r="J30" s="2" t="s">
-        <v>451</v>
+        <v>468</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>550</v>
+        <v>572</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>487</v>
+        <v>532</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="O30" s="2" t="s">
-        <v>738</v>
-      </c>
-      <c r="P30" s="2" t="s">
-        <v>496</v>
-      </c>
-      <c r="Q30" s="2" t="s">
-        <v>490</v>
-      </c>
-      <c r="R30" s="2" t="s">
-        <v>489</v>
+        <v>533</v>
+      </c>
+      <c r="N30" s="82"/>
+      <c r="O30" s="82" t="s">
+        <v>737</v>
+      </c>
+      <c r="P30" s="82" t="s">
+        <v>606</v>
+      </c>
+      <c r="Q30" s="82" t="s">
+        <v>605</v>
+      </c>
+      <c r="R30" s="82" t="s">
+        <v>606</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>578</v>
+        <v>607</v>
       </c>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="2:27" ht="114" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:27" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
-        <v>366</v>
+        <v>377</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>422</v>
+        <v>424</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>413</v>
-      </c>
-      <c r="E31" s="85" t="s">
-        <v>709</v>
+        <v>394</v>
+      </c>
+      <c r="E31" s="2" t="s">
+        <v>711</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>94</v>
+        <v>525</v>
       </c>
       <c r="J31" s="2" t="s">
-        <v>453</v>
+        <v>465</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>550</v>
+        <v>571</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>666</v>
+        <v>526</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>669</v>
+        <v>736</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>670</v>
+        <v>586</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>667</v>
+        <v>518</v>
       </c>
       <c r="R31" s="2" t="s">
-        <v>668</v>
+        <v>489</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>671</v>
+        <v>587</v>
       </c>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:27" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
-        <v>369</v>
+        <v>383</v>
       </c>
       <c r="C32" s="2" t="s">
-        <v>422</v>
+        <v>220</v>
       </c>
       <c r="D32" s="2" t="s">
-        <v>415</v>
+        <v>402</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>718</v>
+        <v>695</v>
       </c>
       <c r="I32" s="2" t="s">
-        <v>476</v>
+        <v>552</v>
       </c>
       <c r="J32" s="2" t="s">
-        <v>452</v>
+        <v>554</v>
       </c>
       <c r="K32" s="2" t="s">
-        <v>452</v>
+        <v>555</v>
       </c>
       <c r="L32" s="2" t="s">
-        <v>499</v>
-      </c>
-      <c r="M32" s="2">
-        <v>1</v>
+        <v>556</v>
+      </c>
+      <c r="M32" s="2" t="s">
+        <v>479</v>
       </c>
       <c r="O32" s="82" t="s">
-        <v>677</v>
-      </c>
-      <c r="P32" s="2" t="s">
-        <v>678</v>
+        <v>721</v>
+      </c>
+      <c r="P32" s="82" t="s">
+        <v>626</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>667</v>
+        <v>514</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>668</v>
+        <v>515</v>
       </c>
       <c r="S32" s="82" t="s">
-        <v>687</v>
+        <v>556</v>
       </c>
       <c r="U32" s="2"/>
     </row>
-    <row r="33" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="1:25" ht="256.5" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
-        <v>409</v>
+        <v>362</v>
       </c>
       <c r="C33" s="2" t="s">
         <v>359</v>
       </c>
       <c r="D33" s="2" t="s">
-        <v>410</v>
+        <v>412</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>701</v>
+        <v>698</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>471</v>
+        <v>654</v>
       </c>
       <c r="J33" s="2" t="s">
-        <v>645</v>
+        <v>473</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="L33" s="2" t="s">
-        <v>646</v>
+        <v>650</v>
+      </c>
+      <c r="L33" s="82" t="s">
+        <v>412</v>
       </c>
       <c r="M33" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>648</v>
+        <v>653</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>574</v>
+        <v>613</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>647</v>
+        <v>651</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>481</v>
+        <v>610</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>649</v>
+        <v>652</v>
       </c>
       <c r="U33" s="2"/>
     </row>
-    <row r="34" spans="2:21" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
-        <v>389</v>
+        <v>363</v>
       </c>
       <c r="C34" s="2" t="s">
-        <v>426</v>
+        <v>424</v>
       </c>
       <c r="D34" s="2" t="s">
-        <v>408</v>
-      </c>
-      <c r="E34" s="2">
-        <v>2</v>
+        <v>432</v>
+      </c>
+      <c r="E34" s="2" t="s">
+        <v>703</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>471</v>
+        <v>548</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>523</v>
+        <v>657</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>572</v>
+        <v>550</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>522</v>
+        <v>658</v>
       </c>
       <c r="M34" s="2">
         <v>1</v>
       </c>
-      <c r="O34" s="2" t="s">
-        <v>739</v>
-      </c>
-      <c r="P34" s="2" t="s">
-        <v>574</v>
-      </c>
-      <c r="Q34" s="2" t="s">
-        <v>524</v>
-      </c>
-      <c r="R34" s="2" t="s">
+      <c r="O34" s="82" t="s">
+        <v>659</v>
+      </c>
+      <c r="P34" s="82" t="s">
+        <v>613</v>
+      </c>
+      <c r="Q34" s="82" t="s">
+        <v>660</v>
+      </c>
+      <c r="R34" s="82" t="s">
         <v>481</v>
       </c>
-      <c r="S34" s="2" t="s">
-        <v>573</v>
+      <c r="S34" s="82" t="s">
+        <v>661</v>
       </c>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="2:21" ht="171" x14ac:dyDescent="0.45">
+    <row r="35" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
-        <v>378</v>
+        <v>382</v>
       </c>
       <c r="C35" s="2" t="s">
-        <v>427</v>
+        <v>424</v>
       </c>
       <c r="D35" s="2" t="s">
-        <v>395</v>
-      </c>
-      <c r="E35" s="2">
-        <v>1</v>
+        <v>399</v>
+      </c>
+      <c r="E35" s="2" t="s">
+        <v>714</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>525</v>
+        <v>553</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>466</v>
+        <v>655</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>546</v>
+        <v>550</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>527</v>
+        <v>656</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>740</v>
+        <v>615</v>
+      </c>
+      <c r="P35" s="2" t="s">
+        <v>547</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>528</v>
+        <v>614</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>529</v>
+        <v>609</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>588</v>
+        <v>612</v>
       </c>
       <c r="U35" s="2"/>
     </row>
-    <row r="36" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="36" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A36" s="86"/>
       <c r="B36" s="2" t="s">
-        <v>377</v>
+        <v>382</v>
       </c>
       <c r="C36" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>394</v>
+        <v>399</v>
       </c>
       <c r="E36" s="2" t="s">
         <v>714</v>
       </c>
+      <c r="F36" s="86"/>
+      <c r="G36" s="86"/>
+      <c r="H36" s="86"/>
       <c r="I36" s="2" t="s">
-        <v>525</v>
+        <v>553</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>465</v>
+        <v>655</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>571</v>
+        <v>550</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>526</v>
+        <v>656</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O36" s="2" t="s">
-        <v>741</v>
-      </c>
-      <c r="P36" s="2" t="s">
-        <v>586</v>
-      </c>
-      <c r="Q36" s="2" t="s">
-        <v>518</v>
-      </c>
-      <c r="R36" s="2" t="s">
-        <v>489</v>
-      </c>
-      <c r="S36" s="2" t="s">
-        <v>587</v>
-      </c>
-      <c r="U36" s="2"/>
-    </row>
-    <row r="37" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="N36" s="86"/>
+      <c r="O36" s="82" t="s">
+        <v>747</v>
+      </c>
+      <c r="P36" s="82" t="s">
+        <v>547</v>
+      </c>
+      <c r="Q36" s="82" t="s">
+        <v>744</v>
+      </c>
+      <c r="R36" s="82" t="s">
+        <v>745</v>
+      </c>
+      <c r="S36" s="82" t="s">
+        <v>746</v>
+      </c>
+      <c r="U36" s="86"/>
+      <c r="V36" s="86"/>
+      <c r="W36" s="86"/>
+      <c r="X36" s="86"/>
+      <c r="Y36" s="86"/>
+    </row>
+    <row r="37" spans="1:25" ht="171" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
-        <v>380</v>
+        <v>372</v>
       </c>
       <c r="C37" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D37" s="2" t="s">
+        <v>404</v>
+      </c>
+      <c r="E37" s="85" t="s">
+        <v>696</v>
+      </c>
+      <c r="I37" s="2" t="s">
+        <v>553</v>
+      </c>
+      <c r="J37" s="2" t="s">
+        <v>461</v>
+      </c>
+      <c r="K37" s="2" t="s">
+        <v>560</v>
+      </c>
+      <c r="L37" s="82" t="s">
+        <v>404</v>
+      </c>
+      <c r="M37" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="O37" s="2" t="s">
+        <v>561</v>
+      </c>
+      <c r="P37" s="82" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q37" s="82" t="s">
+        <v>558</v>
+      </c>
+      <c r="R37" s="82" t="s">
+        <v>559</v>
+      </c>
+      <c r="S37" s="82" t="s">
+        <v>629</v>
+      </c>
+      <c r="U37" s="2"/>
+    </row>
+    <row r="38" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B38" s="2" t="s">
+        <v>401</v>
+      </c>
+      <c r="C38" s="2" t="s">
         <v>424</v>
       </c>
-      <c r="D37" s="2" t="s">
-        <v>397</v>
-      </c>
-      <c r="E37" s="84">
-        <v>0.6020833333333333</v>
-      </c>
-      <c r="I37" s="2" t="s">
-        <v>530</v>
-      </c>
-      <c r="J37" s="2" t="s">
-        <v>468</v>
-      </c>
-      <c r="K37" s="2" t="s">
-        <v>572</v>
-      </c>
-      <c r="L37" s="2" t="s">
-        <v>532</v>
-      </c>
-      <c r="M37" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="N37" s="82"/>
-      <c r="O37" s="82" t="s">
-        <v>742</v>
-      </c>
-      <c r="P37" s="82" t="s">
-        <v>606</v>
-      </c>
-      <c r="Q37" s="82" t="s">
-        <v>605</v>
-      </c>
-      <c r="R37" s="82" t="s">
-        <v>606</v>
-      </c>
-      <c r="S37" s="2" t="s">
-        <v>607</v>
-      </c>
-      <c r="U37" s="2"/>
-    </row>
-    <row r="38" spans="2:21" ht="256.5" x14ac:dyDescent="0.45">
-      <c r="B38" s="2" t="s">
-        <v>362</v>
-      </c>
-      <c r="C38" s="2" t="s">
-        <v>359</v>
-      </c>
       <c r="D38" s="2" t="s">
-        <v>412</v>
+        <v>400</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>701</v>
+        <v>714</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>655</v>
+        <v>548</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>473</v>
+        <v>549</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="L38" s="82" t="s">
-        <v>412</v>
+        <v>550</v>
+      </c>
+      <c r="L38" s="2" t="s">
+        <v>551</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O38" s="2" t="s">
-        <v>654</v>
-      </c>
-      <c r="P38" s="2" t="s">
-        <v>613</v>
-      </c>
-      <c r="Q38" s="2" t="s">
-        <v>652</v>
-      </c>
-      <c r="R38" s="2" t="s">
-        <v>610</v>
-      </c>
-      <c r="S38" s="2" t="s">
-        <v>653</v>
+      <c r="O38" s="82" t="s">
+        <v>618</v>
+      </c>
+      <c r="P38" s="82" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q38" s="82" t="s">
+        <v>614</v>
+      </c>
+      <c r="R38" s="82" t="s">
+        <v>609</v>
+      </c>
+      <c r="S38" s="82" t="s">
+        <v>612</v>
       </c>
       <c r="U38" s="2"/>
     </row>
-    <row r="39" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="39" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A39" s="86"/>
       <c r="B39" s="2" t="s">
-        <v>363</v>
+        <v>401</v>
       </c>
       <c r="C39" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D39" s="2" t="s">
-        <v>432</v>
+        <v>400</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>706</v>
-      </c>
+        <v>714</v>
+      </c>
+      <c r="F39" s="86"/>
+      <c r="G39" s="86"/>
+      <c r="H39" s="86"/>
       <c r="I39" s="2" t="s">
         <v>548</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>658</v>
+        <v>549</v>
       </c>
       <c r="K39" s="2" t="s">
         <v>550</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>659</v>
-      </c>
-      <c r="M39" s="2">
-        <v>1</v>
-      </c>
+        <v>551</v>
+      </c>
+      <c r="M39" s="2" t="s">
+        <v>479</v>
+      </c>
+      <c r="N39" s="86"/>
       <c r="O39" s="82" t="s">
-        <v>660</v>
+        <v>743</v>
       </c>
       <c r="P39" s="82" t="s">
-        <v>613</v>
+        <v>547</v>
       </c>
       <c r="Q39" s="82" t="s">
-        <v>661</v>
+        <v>744</v>
       </c>
       <c r="R39" s="82" t="s">
-        <v>481</v>
+        <v>745</v>
       </c>
       <c r="S39" s="82" t="s">
-        <v>662</v>
-      </c>
-      <c r="U39" s="2"/>
-    </row>
-    <row r="40" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+        <v>746</v>
+      </c>
+      <c r="U39" s="86"/>
+      <c r="V39" s="86"/>
+      <c r="W39" s="86"/>
+      <c r="X39" s="86"/>
+      <c r="Y39" s="86"/>
+    </row>
+    <row r="40" spans="1:25" ht="313.5" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
-        <v>382</v>
+        <v>361</v>
       </c>
       <c r="C40" s="2" t="s">
-        <v>424</v>
+        <v>425</v>
       </c>
       <c r="D40" s="2" t="s">
-        <v>399</v>
-      </c>
-      <c r="E40" s="2" t="s">
-        <v>717</v>
+        <v>411</v>
+      </c>
+      <c r="E40" s="85" t="s">
+        <v>702</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>553</v>
+        <v>649</v>
       </c>
       <c r="J40" s="2" t="s">
-        <v>656</v>
+        <v>472</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="L40" s="2" t="s">
-        <v>657</v>
+        <v>650</v>
+      </c>
+      <c r="L40" s="82" t="s">
+        <v>686</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O40" s="2" t="s">
-        <v>615</v>
-      </c>
-      <c r="P40" s="2" t="s">
-        <v>547</v>
-      </c>
-      <c r="Q40" s="2" t="s">
-        <v>614</v>
-      </c>
-      <c r="R40" s="2" t="s">
+      <c r="O40" s="82" t="s">
+        <v>617</v>
+      </c>
+      <c r="P40" s="82" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q40" s="82" t="s">
+        <v>608</v>
+      </c>
+      <c r="R40" s="82" t="s">
         <v>609</v>
       </c>
-      <c r="S40" s="2" t="s">
-        <v>612</v>
+      <c r="S40" s="82" t="s">
+        <v>611</v>
       </c>
       <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="2:21" ht="171" x14ac:dyDescent="0.45">
+    <row r="41" spans="1:25" ht="356.25" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
-        <v>372</v>
+        <v>387</v>
       </c>
       <c r="C41" s="2" t="s">
-        <v>220</v>
+        <v>424</v>
       </c>
       <c r="D41" s="2" t="s">
-        <v>404</v>
+        <v>431</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>699</v>
+        <v>700</v>
       </c>
       <c r="I41" s="2" t="s">
-        <v>553</v>
+        <v>470</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>461</v>
+        <v>639</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>560</v>
-      </c>
-      <c r="L41" s="82" t="s">
-        <v>404</v>
-      </c>
-      <c r="M41" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="O41" s="2" t="s">
-        <v>561</v>
+        <v>550</v>
+      </c>
+      <c r="L41" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="M41" s="2">
+        <v>1</v>
+      </c>
+      <c r="O41" s="82" t="s">
+        <v>738</v>
       </c>
       <c r="P41" s="82" t="s">
-        <v>628</v>
+        <v>640</v>
       </c>
       <c r="Q41" s="82" t="s">
-        <v>558</v>
+        <v>518</v>
       </c>
       <c r="R41" s="82" t="s">
-        <v>559</v>
+        <v>489</v>
       </c>
       <c r="S41" s="82" t="s">
-        <v>629</v>
+        <v>642</v>
       </c>
       <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="42" spans="1:25" ht="285" x14ac:dyDescent="0.45">
       <c r="B42" s="2" t="s">
-        <v>401</v>
+        <v>388</v>
       </c>
       <c r="C42" s="2" t="s">
         <v>424</v>
       </c>
       <c r="D42" s="2" t="s">
-        <v>400</v>
-      </c>
-      <c r="E42" s="2" t="s">
-        <v>717</v>
+        <v>407</v>
+      </c>
+      <c r="E42" s="85" t="s">
+        <v>701</v>
       </c>
       <c r="I42" s="2" t="s">
-        <v>548</v>
+        <v>470</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>549</v>
+        <v>639</v>
       </c>
       <c r="K42" s="2" t="s">
         <v>550</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>551</v>
-      </c>
-      <c r="M42" s="2" t="s">
+        <v>638</v>
+      </c>
+      <c r="M42" s="2">
+        <v>1</v>
+      </c>
+      <c r="O42" s="82" t="s">
+        <v>738</v>
+      </c>
+      <c r="P42" s="82" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q42" s="82" t="s">
+        <v>518</v>
+      </c>
+      <c r="R42" s="82" t="s">
+        <v>489</v>
+      </c>
+      <c r="S42" s="82" t="s">
+        <v>642</v>
+      </c>
+      <c r="U42" s="2"/>
+    </row>
+    <row r="43" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B43" s="2" t="s">
+        <v>360</v>
+      </c>
+      <c r="C43" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D43" s="2" t="s">
+        <v>462</v>
+      </c>
+      <c r="E43" s="2" t="s">
+        <v>698</v>
+      </c>
+      <c r="I43" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="J43" s="2" t="s">
+        <v>469</v>
+      </c>
+      <c r="K43" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="L43" s="2" t="s">
+        <v>643</v>
+      </c>
+      <c r="M43" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="O43" s="82" t="s">
+        <v>738</v>
+      </c>
+      <c r="P43" s="82" t="s">
+        <v>640</v>
+      </c>
+      <c r="Q43" s="82" t="s">
+        <v>518</v>
+      </c>
+      <c r="R43" s="82" t="s">
+        <v>489</v>
+      </c>
+      <c r="S43" s="82" t="s">
+        <v>642</v>
+      </c>
+      <c r="U43" s="2"/>
+    </row>
+    <row r="44" spans="1:25" ht="399" x14ac:dyDescent="0.45">
+      <c r="B44" s="2" t="s">
+        <v>386</v>
+      </c>
+      <c r="C44" s="2" t="s">
+        <v>359</v>
+      </c>
+      <c r="D44" s="2" t="s">
+        <v>406</v>
+      </c>
+      <c r="E44" s="2" t="s">
+        <v>699</v>
+      </c>
+      <c r="I44" s="2" t="s">
+        <v>470</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>637</v>
+      </c>
+      <c r="K44" s="2" t="s">
+        <v>572</v>
+      </c>
+      <c r="L44" s="2" t="s">
+        <v>636</v>
+      </c>
+      <c r="M44" s="2">
+        <v>1</v>
+      </c>
+      <c r="O44" s="82" t="s">
+        <v>739</v>
+      </c>
+      <c r="P44" s="82" t="s">
+        <v>641</v>
+      </c>
+      <c r="Q44" s="82" t="s">
+        <v>635</v>
+      </c>
+      <c r="R44" s="82" t="s">
+        <v>481</v>
+      </c>
+      <c r="S44" s="82" t="s">
+        <v>636</v>
+      </c>
+      <c r="U44" s="2"/>
+    </row>
+    <row r="45" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B45" s="2" t="s">
+        <v>365</v>
+      </c>
+      <c r="C45" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D45" s="2" t="s">
+        <v>464</v>
+      </c>
+      <c r="E45" s="2" t="s">
+        <v>705</v>
+      </c>
+      <c r="I45" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="J45" s="2" t="s">
+        <v>460</v>
+      </c>
+      <c r="K45" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="L45" s="82" t="s">
+        <v>464</v>
+      </c>
+      <c r="M45" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="O45" s="2" t="s">
+        <v>740</v>
+      </c>
+      <c r="P45" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="Q45" s="2" t="s">
+        <v>663</v>
+      </c>
+      <c r="R45" s="2" t="s">
+        <v>481</v>
+      </c>
+      <c r="S45" s="82" t="s">
+        <v>464</v>
+      </c>
+      <c r="U45" s="2"/>
+    </row>
+    <row r="46" spans="1:25" ht="99.75" x14ac:dyDescent="0.45">
+      <c r="B46" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C46" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D46" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E46" s="85" t="s">
+        <v>697</v>
+      </c>
+      <c r="I46" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>564</v>
+      </c>
+      <c r="K46" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="L46" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="M46" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O42" s="82" t="s">
-        <v>618</v>
-      </c>
-      <c r="P42" s="82" t="s">
-        <v>616</v>
-      </c>
-      <c r="Q42" s="82" t="s">
-        <v>614</v>
-      </c>
-      <c r="R42" s="82" t="s">
-        <v>609</v>
-      </c>
-      <c r="S42" s="82" t="s">
-        <v>612</v>
-      </c>
-      <c r="U42" s="2"/>
-    </row>
-    <row r="43" spans="2:21" ht="313.5" x14ac:dyDescent="0.45">
-      <c r="B43" s="2" t="s">
-        <v>361</v>
-      </c>
-      <c r="C43" s="2" t="s">
-        <v>425</v>
-      </c>
-      <c r="D43" s="2" t="s">
-        <v>411</v>
-      </c>
-      <c r="E43" s="85" t="s">
-        <v>705</v>
-      </c>
-      <c r="I43" s="2" t="s">
-        <v>650</v>
-      </c>
-      <c r="J43" s="2" t="s">
-        <v>472</v>
-      </c>
-      <c r="K43" s="2" t="s">
-        <v>651</v>
-      </c>
-      <c r="L43" s="82" t="s">
-        <v>688</v>
-      </c>
-      <c r="M43" s="2" t="s">
+      <c r="O46" s="82" t="s">
+        <v>631</v>
+      </c>
+      <c r="P46" s="82" t="s">
+        <v>634</v>
+      </c>
+      <c r="Q46" s="82" t="s">
+        <v>633</v>
+      </c>
+      <c r="R46" s="82" t="s">
+        <v>610</v>
+      </c>
+      <c r="S46" s="82" t="s">
+        <v>632</v>
+      </c>
+      <c r="U46" s="2"/>
+    </row>
+    <row r="47" spans="1:25" ht="57" x14ac:dyDescent="0.45">
+      <c r="B47" s="2" t="s">
+        <v>385</v>
+      </c>
+      <c r="C47" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D47" s="2" t="s">
+        <v>405</v>
+      </c>
+      <c r="E47" s="85" t="s">
+        <v>697</v>
+      </c>
+      <c r="I47" s="2" t="s">
+        <v>563</v>
+      </c>
+      <c r="J47" s="2" t="s">
+        <v>562</v>
+      </c>
+      <c r="K47" s="2" t="s">
+        <v>555</v>
+      </c>
+      <c r="L47" s="82" t="s">
+        <v>405</v>
+      </c>
+      <c r="M47" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="O43" s="82" t="s">
-        <v>617</v>
-      </c>
-      <c r="P43" s="82" t="s">
-        <v>616</v>
-      </c>
-      <c r="Q43" s="82" t="s">
-        <v>608</v>
-      </c>
-      <c r="R43" s="82" t="s">
-        <v>609</v>
-      </c>
-      <c r="S43" s="82" t="s">
-        <v>611</v>
-      </c>
-      <c r="U43" s="2"/>
-    </row>
-    <row r="44" spans="2:21" ht="99.75" x14ac:dyDescent="0.45">
-      <c r="B44" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C44" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D44" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E44" s="85" t="s">
-        <v>700</v>
-      </c>
-      <c r="I44" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="J44" s="2" t="s">
-        <v>564</v>
-      </c>
-      <c r="K44" s="2" t="s">
+      <c r="O47" s="82" t="s">
+        <v>630</v>
+      </c>
+      <c r="P47" s="82" t="s">
+        <v>628</v>
+      </c>
+      <c r="Q47" s="82" t="s">
+        <v>558</v>
+      </c>
+      <c r="R47" s="82" t="s">
+        <v>559</v>
+      </c>
+      <c r="S47" s="82" t="s">
+        <v>629</v>
+      </c>
+      <c r="U47" s="2"/>
+    </row>
+    <row r="48" spans="1:25" ht="199.5" x14ac:dyDescent="0.45">
+      <c r="B48" s="2" t="s">
+        <v>364</v>
+      </c>
+      <c r="C48" s="2" t="s">
+        <v>424</v>
+      </c>
+      <c r="D48" s="2" t="s">
+        <v>463</v>
+      </c>
+      <c r="E48" s="2" t="s">
+        <v>704</v>
+      </c>
+      <c r="I48" s="82" t="s">
+        <v>548</v>
+      </c>
+      <c r="J48" s="82" t="s">
+        <v>684</v>
+      </c>
+      <c r="K48" s="82" t="s">
         <v>550</v>
       </c>
-      <c r="L44" s="82" t="s">
-        <v>405</v>
-      </c>
-      <c r="M44" s="2" t="s">
+      <c r="L48" s="82" t="s">
+        <v>463</v>
+      </c>
+      <c r="M48" s="82" t="s">
         <v>479</v>
       </c>
-      <c r="O44" s="82" t="s">
-        <v>631</v>
-      </c>
-      <c r="P44" s="82" t="s">
-        <v>634</v>
-      </c>
-      <c r="Q44" s="82" t="s">
-        <v>633</v>
-      </c>
-      <c r="R44" s="82" t="s">
-        <v>610</v>
-      </c>
-      <c r="S44" s="82" t="s">
-        <v>632</v>
-      </c>
-      <c r="U44" s="2"/>
-    </row>
-    <row r="45" spans="2:21" ht="57" x14ac:dyDescent="0.45">
-      <c r="B45" s="2" t="s">
-        <v>385</v>
-      </c>
-      <c r="C45" s="2" t="s">
-        <v>220</v>
-      </c>
-      <c r="D45" s="2" t="s">
-        <v>405</v>
-      </c>
-      <c r="E45" s="85" t="s">
-        <v>700</v>
-      </c>
-      <c r="I45" s="2" t="s">
-        <v>563</v>
-      </c>
-      <c r="J45" s="2" t="s">
-        <v>562</v>
-      </c>
-      <c r="K45" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="L45" s="82" t="s">
-        <v>405</v>
-      </c>
-      <c r="M45" s="2" t="s">
-        <v>479</v>
-      </c>
-      <c r="O45" s="82" t="s">
-        <v>630</v>
-      </c>
-      <c r="P45" s="82" t="s">
-        <v>628</v>
-      </c>
-      <c r="Q45" s="82" t="s">
-        <v>558</v>
-      </c>
-      <c r="R45" s="82" t="s">
-        <v>559</v>
-      </c>
-      <c r="S45" s="82" t="s">
-        <v>629</v>
-      </c>
-      <c r="U45" s="2"/>
-    </row>
-    <row r="46" spans="2:21" ht="199.5" x14ac:dyDescent="0.45">
-      <c r="B46" s="2" t="s">
-        <v>364</v>
-      </c>
-      <c r="C46" s="2" t="s">
-        <v>424</v>
-      </c>
-      <c r="D46" s="2" t="s">
-        <v>463</v>
-      </c>
-      <c r="E46" s="2" t="s">
-        <v>707</v>
-      </c>
-      <c r="I46" s="82" t="s">
-        <v>548</v>
-      </c>
-      <c r="J46" s="82" t="s">
-        <v>686</v>
-      </c>
-      <c r="K46" s="82" t="s">
-        <v>550</v>
-      </c>
-      <c r="L46" s="82" t="s">
-        <v>463</v>
-      </c>
-      <c r="M46" s="82" t="s">
-        <v>479</v>
-      </c>
-      <c r="O46" s="82" t="s">
+      <c r="O48" s="82" t="s">
+        <v>680</v>
+      </c>
+      <c r="P48" s="82" t="s">
+        <v>681</v>
+      </c>
+      <c r="Q48" s="82" t="s">
         <v>682</v>
       </c>
-      <c r="P46" s="82" t="s">
+      <c r="R48" s="82" t="s">
+        <v>481</v>
+      </c>
+      <c r="S48" s="82" t="s">
         <v>683</v>
       </c>
-      <c r="Q46" s="82" t="s">
-        <v>684</v>
-      </c>
-      <c r="R46" s="82" t="s">
-        <v>481</v>
-      </c>
-      <c r="S46" s="82" t="s">
-        <v>685</v>
-      </c>
-      <c r="U46" s="2"/>
+      <c r="U48" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W47:W1048576 V2:V46" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W49:W1048576 V2:V48" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
     <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">

</xml_diff>

<commit_message>
Moved j:CourtOrder, j:Conviction, j:SentenceModification, j:SubjectAssignment under j:Sentence
</commit_message>
<xml_diff>
--- a/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
+++ b/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformCommitmentOrder_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64F21CD0-9262-485F-AC88-D40F3A0BF03F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{7EF8D392-5DD6-4713-97F1-5BC523C15708}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-4065" yWindow="-21600" windowWidth="26025" windowHeight="20985" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-98" yWindow="-98" windowWidth="21795" windowHeight="13875" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -140,7 +140,6 @@
     <definedName name="Type_Target_Style">Type!$L$1</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
-  <fileRecoveryPr repairLoad="1"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
       <xcalcf:calcFeatures>
@@ -3468,7 +3467,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3699,9 +3698,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7628,17 +7624,18 @@
   <dimension ref="A1:AA48"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C40" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C42" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="E40" sqref="E40"/>
+      <selection pane="bottomRight" activeCell="E39" sqref="E39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
   <cols>
     <col min="1" max="1" width="11.6640625" style="2" hidden="1" customWidth="1"/>
     <col min="2" max="2" width="16.59765625" style="2" customWidth="1"/>
-    <col min="3" max="4" width="7.265625" style="2" customWidth="1"/>
+    <col min="3" max="3" width="7.265625" style="2" customWidth="1"/>
+    <col min="4" max="4" width="15.73046875" style="2" customWidth="1"/>
     <col min="5" max="5" width="17.19921875" style="2" customWidth="1"/>
     <col min="6" max="6" width="4.9296875" style="2" hidden="1" customWidth="1"/>
     <col min="7" max="8" width="22.6640625" style="2" hidden="1" customWidth="1"/>
@@ -9177,7 +9174,7 @@
       </c>
       <c r="U32" s="2"/>
     </row>
-    <row r="33" spans="1:25" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:21" ht="256.5" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
         <v>362</v>
       </c>
@@ -9222,7 +9219,7 @@
       </c>
       <c r="U33" s="2"/>
     </row>
-    <row r="34" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
         <v>363</v>
       </c>
@@ -9267,7 +9264,7 @@
       </c>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
         <v>382</v>
       </c>
@@ -9312,8 +9309,7 @@
       </c>
       <c r="U35" s="2"/>
     </row>
-    <row r="36" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A36" s="86"/>
+    <row r="36" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B36" s="2" t="s">
         <v>382</v>
       </c>
@@ -9326,9 +9322,6 @@
       <c r="E36" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="F36" s="86"/>
-      <c r="G36" s="86"/>
-      <c r="H36" s="86"/>
       <c r="I36" s="2" t="s">
         <v>553</v>
       </c>
@@ -9344,7 +9337,6 @@
       <c r="M36" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="N36" s="86"/>
       <c r="O36" s="82" t="s">
         <v>747</v>
       </c>
@@ -9360,13 +9352,9 @@
       <c r="S36" s="82" t="s">
         <v>746</v>
       </c>
-      <c r="U36" s="86"/>
-      <c r="V36" s="86"/>
-      <c r="W36" s="86"/>
-      <c r="X36" s="86"/>
-      <c r="Y36" s="86"/>
-    </row>
-    <row r="37" spans="1:25" ht="171" x14ac:dyDescent="0.45">
+      <c r="U36" s="2"/>
+    </row>
+    <row r="37" spans="2:21" ht="171" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
         <v>372</v>
       </c>
@@ -9411,7 +9399,7 @@
       </c>
       <c r="U37" s="2"/>
     </row>
-    <row r="38" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="38" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B38" s="2" t="s">
         <v>401</v>
       </c>
@@ -9456,8 +9444,7 @@
       </c>
       <c r="U38" s="2"/>
     </row>
-    <row r="39" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A39" s="86"/>
+    <row r="39" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B39" s="2" t="s">
         <v>401</v>
       </c>
@@ -9470,9 +9457,6 @@
       <c r="E39" s="2" t="s">
         <v>714</v>
       </c>
-      <c r="F39" s="86"/>
-      <c r="G39" s="86"/>
-      <c r="H39" s="86"/>
       <c r="I39" s="2" t="s">
         <v>548</v>
       </c>
@@ -9488,7 +9472,6 @@
       <c r="M39" s="2" t="s">
         <v>479</v>
       </c>
-      <c r="N39" s="86"/>
       <c r="O39" s="82" t="s">
         <v>743</v>
       </c>
@@ -9504,13 +9487,9 @@
       <c r="S39" s="82" t="s">
         <v>746</v>
       </c>
-      <c r="U39" s="86"/>
-      <c r="V39" s="86"/>
-      <c r="W39" s="86"/>
-      <c r="X39" s="86"/>
-      <c r="Y39" s="86"/>
-    </row>
-    <row r="40" spans="1:25" ht="313.5" x14ac:dyDescent="0.45">
+      <c r="U39" s="2"/>
+    </row>
+    <row r="40" spans="2:21" ht="313.5" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
         <v>361</v>
       </c>
@@ -9555,7 +9534,7 @@
       </c>
       <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="1:25" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:21" ht="356.25" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
         <v>387</v>
       </c>
@@ -9600,7 +9579,7 @@
       </c>
       <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="1:25" ht="285" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:21" ht="285" x14ac:dyDescent="0.45">
       <c r="B42" s="2" t="s">
         <v>388</v>
       </c>
@@ -9645,7 +9624,7 @@
       </c>
       <c r="U42" s="2"/>
     </row>
-    <row r="43" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="43" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B43" s="2" t="s">
         <v>360</v>
       </c>
@@ -9690,7 +9669,7 @@
       </c>
       <c r="U43" s="2"/>
     </row>
-    <row r="44" spans="1:25" ht="399" x14ac:dyDescent="0.45">
+    <row r="44" spans="2:21" ht="399" x14ac:dyDescent="0.45">
       <c r="B44" s="2" t="s">
         <v>386</v>
       </c>
@@ -9735,7 +9714,7 @@
       </c>
       <c r="U44" s="2"/>
     </row>
-    <row r="45" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="45" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
       <c r="B45" s="2" t="s">
         <v>365</v>
       </c>
@@ -9780,7 +9759,7 @@
       </c>
       <c r="U45" s="2"/>
     </row>
-    <row r="46" spans="1:25" ht="99.75" x14ac:dyDescent="0.45">
+    <row r="46" spans="2:21" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B46" s="2" t="s">
         <v>385</v>
       </c>
@@ -9825,7 +9804,7 @@
       </c>
       <c r="U46" s="2"/>
     </row>
-    <row r="47" spans="1:25" ht="57" x14ac:dyDescent="0.45">
+    <row r="47" spans="2:21" ht="57" x14ac:dyDescent="0.45">
       <c r="B47" s="2" t="s">
         <v>385</v>
       </c>
@@ -9870,7 +9849,7 @@
       </c>
       <c r="U47" s="2"/>
     </row>
-    <row r="48" spans="1:25" ht="199.5" x14ac:dyDescent="0.45">
+    <row r="48" spans="2:21" ht="199.5" x14ac:dyDescent="0.45">
       <c r="B48" s="2" t="s">
         <v>364</v>
       </c>

</xml_diff>

<commit_message>
Added ChargeKey, multiple charge example
</commit_message>
<xml_diff>
--- a/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
+++ b/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformCommitmentOrder_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CB8A672F-2121-4EB6-A22A-5E0478A84319}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC437EF-38F3-41A9-BDBB-89B0A3CD6848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="12030" yWindow="-21135" windowWidth="16200" windowHeight="19890" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="13335" yWindow="-21225" windowWidth="22755" windowHeight="19890" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -26,7 +26,7 @@
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="6" hidden="1">'Codes | Facets'!$A$1:$M$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="7">Namespace!$A$1:$N$1</definedName>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$48</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="3" hidden="1">Property!$A$1:$V$49</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="4">Type!$A$1:$L$1</definedName>
     <definedName name="_xlnm._FilterDatabase" localSheetId="5">'Type-Has-Property'!$A$1:$P$1</definedName>
     <definedName name="CODES_NamespaceStyle">'Field Descriptions'!$B$165:$B$176</definedName>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1211" uniqueCount="753">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="760">
   <si>
     <t>Definition</t>
   </si>
@@ -3123,6 +3123,27 @@
   </si>
   <si>
     <t>SentenceCode</t>
+  </si>
+  <si>
+    <t>ChargeKey</t>
+  </si>
+  <si>
+    <t>String</t>
+  </si>
+  <si>
+    <t>A unique identifer that is to be stored as a Key in each endpoint system's statute code or charge table</t>
+  </si>
+  <si>
+    <t>A UCT Charge Key (Uniform Charge Table) is a shared key or identifier from a shared table that standardizes charge code definitions across the enterprise.</t>
+  </si>
+  <si>
+    <t>j:Charge/nola-ext:ChargeAugmentation/nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeAugmentationType</t>
+  </si>
+  <si>
+    <t>nola-ext:ChargeKey</t>
   </si>
 </sst>
 </file>
@@ -3482,7 +3503,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="86">
+  <cellXfs count="87">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3715,6 +3736,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
   </cellXfs>
   <cellStyles count="71">
     <cellStyle name="Accent1" xfId="1" builtinId="29"/>
@@ -4980,8 +5004,8 @@
 </file>
 
 <file path=xl/tables/table6.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y48" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
-  <autoFilter ref="A1:Y48" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{00000000-000C-0000-FFFF-FFFF05000000}" name="Table3" displayName="Table3" ref="A1:Y49" totalsRowShown="0" headerRowDxfId="106" dataDxfId="105" headerRowCellStyle="Accent2">
+  <autoFilter ref="A1:Y49" xr:uid="{00000000-0009-0000-0100-000003000000}"/>
   <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="A2:Y48">
     <sortCondition ref="O1:O48"/>
   </sortState>
@@ -7636,13 +7660,13 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
-  <dimension ref="A1:AA48"/>
+  <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C35" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="L36" sqref="L36"/>
+      <selection pane="bottomRight" activeCell="O49" sqref="O49"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -9504,7 +9528,7 @@
       </c>
       <c r="U39" s="2"/>
     </row>
-    <row r="40" spans="2:21" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="40" spans="2:21" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B40" s="2" t="s">
         <v>361</v>
       </c>
@@ -9549,7 +9573,7 @@
       </c>
       <c r="U40" s="2"/>
     </row>
-    <row r="41" spans="2:21" ht="356.25" x14ac:dyDescent="0.45">
+    <row r="41" spans="2:21" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B41" s="2" t="s">
         <v>387</v>
       </c>
@@ -9594,7 +9618,7 @@
       </c>
       <c r="U41" s="2"/>
     </row>
-    <row r="42" spans="2:21" ht="285" x14ac:dyDescent="0.45">
+    <row r="42" spans="2:21" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B42" s="2" t="s">
         <v>388</v>
       </c>
@@ -9908,15 +9932,76 @@
         <v>683</v>
       </c>
       <c r="U48" s="2"/>
+    </row>
+    <row r="49" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="A49" s="86"/>
+      <c r="B49" s="86" t="s">
+        <v>753</v>
+      </c>
+      <c r="C49" s="86" t="s">
+        <v>754</v>
+      </c>
+      <c r="D49" s="2" t="s">
+        <v>755</v>
+      </c>
+      <c r="E49" s="86">
+        <v>1125</v>
+      </c>
+      <c r="F49" s="86">
+        <v>1125</v>
+      </c>
+      <c r="G49" s="86"/>
+      <c r="H49" s="86"/>
+      <c r="I49" s="2" t="s">
+        <v>525</v>
+      </c>
+      <c r="J49" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="K49" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="L49" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="M49" s="2">
+        <v>1</v>
+      </c>
+      <c r="N49" s="86" t="s">
+        <v>479</v>
+      </c>
+      <c r="O49" s="2" t="s">
+        <v>757</v>
+      </c>
+      <c r="P49" s="86" t="s">
+        <v>758</v>
+      </c>
+      <c r="Q49" s="86" t="s">
+        <v>759</v>
+      </c>
+      <c r="R49" s="86" t="s">
+        <v>489</v>
+      </c>
+      <c r="S49" s="86" t="s">
+        <v>756</v>
+      </c>
+      <c r="T49" s="2" t="s">
+        <v>756</v>
+      </c>
+      <c r="U49" s="86"/>
+      <c r="V49" s="86"/>
+      <c r="W49" s="86"/>
+      <c r="X49" s="86"/>
+      <c r="Y49" s="86"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>
   <dataValidations count="3">
     <dataValidation errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F1" xr:uid="{00000000-0002-0000-0300-000000000000}"/>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W49:W1048576 V2:V48" xr:uid="{00000000-0002-0000-0300-000002000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" errorTitle="Invalid value" error="Valid property styles are &quot;element&quot;, &quot;attribute&quot;, or &quot;abstract&quot;.  Leave the cell blank to use the default value &quot;element&quot;." promptTitle="Property Style" prompt="- &quot;element&quot; or blank (default) - Represents a typical NIEM property._x000a_- &quot;abstract&quot; - Used to create a substitution group_x000a_- &quot;attribute&quot; - Use sparingly, if at all; for values tightly-coupled to an element." sqref="W49:W1048576 V2:V49" xr:uid="{00000000-0002-0000-0300-000002000000}">
       <formula1>"element,attribute,abstract"</formula1>
     </dataValidation>
-    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576" xr:uid="{00000000-0002-0000-0300-000001000000}">
+    <dataValidation type="list" errorStyle="information" allowBlank="1" showInputMessage="1" showErrorMessage="1" sqref="F2:F1048576 G49" xr:uid="{00000000-0002-0000-0300-000001000000}">
       <formula1>MAPPING_CODES</formula1>
     </dataValidation>
   </dataValidations>

</xml_diff>

<commit_message>
Replaced person race and sex with NCIC codes, replaced drug used with UCR code
</commit_message>
<xml_diff>
--- a/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
+++ b/schemas/UniformCommitmentOrder_iepd/artifacts/UniformCommitmentOrder_MappingSpreadsheet.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\JamesCabral\git\JTMP-Data-Exchange-Specs\schemas\UniformCommitmentOrder_iepd\artifacts\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4EC437EF-38F3-41A9-BDBB-89B0A3CD6848}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{073DC0CD-32E5-4178-90F2-CAF1F1B0A82D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="13335" yWindow="-21225" windowWidth="22755" windowHeight="19890" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="18225" yWindow="-20775" windowWidth="16920" windowHeight="17730" tabRatio="781" firstSheet="3" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Readme" sheetId="9" state="hidden" r:id="rId1"/>
@@ -160,7 +160,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="760">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1225" uniqueCount="763">
   <si>
     <t>Definition</t>
   </si>
@@ -2387,21 +2387,9 @@
     <t>A classification of a person based on factors such as geographical locations and genetics.</t>
   </si>
   <si>
-    <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/j:PersonRaceText</t>
-  </si>
-  <si>
-    <t>nc:PersonRaceText</t>
-  </si>
-  <si>
-    <t>nc:PersonSexText</t>
-  </si>
-  <si>
     <t>A gender or sex of a person.</t>
   </si>
   <si>
-    <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/j:PersonSexText</t>
-  </si>
-  <si>
     <t>PersonIdentifiers</t>
   </si>
   <si>
@@ -3041,15 +3029,9 @@
     <t>j:CourtOrder/nola-ext:CourtOrderAugmentation/nc:Case/j:CaseAugmentation/j:CaseCourtEvent/nc:ActivityDate/nc:DateTime</t>
   </si>
   <si>
-    <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/hs:PersonAugmentation/hs:HealthDetails/hs:SubstanceAbuseDetails/nc:Substance/nc:SubstanceCategoryText</t>
-  </si>
-  <si>
     <t>nc:SubstanceType</t>
   </si>
   <si>
-    <t>nc:SubstanceCategoryText</t>
-  </si>
-  <si>
     <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/nc:PersonName/nc:PersonFullName</t>
   </si>
   <si>
@@ -3144,6 +3126,33 @@
   </si>
   <si>
     <t>nola-ext:ChargeKey</t>
+  </si>
+  <si>
+    <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/hs:PersonAugmentation/hs:HealthDetails/hs:SubstanceAbuseDetails/nc:Substance/j:DrugCategoryCode</t>
+  </si>
+  <si>
+    <t>j:DrugCategoryCode</t>
+  </si>
+  <si>
+    <t>ucr:DrugCategoryCodeType</t>
+  </si>
+  <si>
+    <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/ncic:PersonSexCode</t>
+  </si>
+  <si>
+    <t>j:CourtOrder/j:CourtOrderDesignatedSubject/nc:RoleOfPerson/ncic:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>ncic:PersonRaceCode</t>
+  </si>
+  <si>
+    <t>ncic:PersonSexCode</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncic:RACECodeType </t>
+  </si>
+  <si>
+    <t xml:space="preserve">ncic:SEXCodeType </t>
   </si>
 </sst>
 </file>
@@ -3287,6 +3296,7 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
     <font>
@@ -3503,7 +3513,7 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="87">
+  <cellXfs count="86">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="2" applyFont="1" applyAlignment="1">
       <alignment wrapText="1"/>
@@ -3734,9 +3744,6 @@
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
   </cellXfs>
@@ -7663,10 +7670,10 @@
   <dimension ref="A1:AA49"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="85" zoomScaleNormal="85" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C48" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="I4" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="O49" sqref="O49"/>
+      <selection pane="bottomRight" activeCell="J5" sqref="J5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.86328125" defaultRowHeight="14.25" x14ac:dyDescent="0.45"/>
@@ -7711,7 +7718,7 @@
         <v>0</v>
       </c>
       <c r="E1" s="3" t="s">
-        <v>687</v>
+        <v>683</v>
       </c>
       <c r="F1" s="9" t="s">
         <v>49</v>
@@ -7729,37 +7736,37 @@
         <v>486</v>
       </c>
       <c r="K1" s="9" t="s">
-        <v>543</v>
+        <v>539</v>
       </c>
       <c r="L1" s="9" t="s">
-        <v>544</v>
+        <v>540</v>
       </c>
       <c r="M1" s="9" t="s">
-        <v>545</v>
+        <v>541</v>
       </c>
       <c r="N1" s="11" t="s">
         <v>48</v>
       </c>
       <c r="O1" s="1" t="s">
+        <v>615</v>
+      </c>
+      <c r="P1" s="11" t="s">
+        <v>616</v>
+      </c>
+      <c r="Q1" s="1" t="s">
+        <v>617</v>
+      </c>
+      <c r="R1" s="1" t="s">
+        <v>618</v>
+      </c>
+      <c r="S1" s="1" t="s">
         <v>619</v>
-      </c>
-      <c r="P1" s="11" t="s">
-        <v>620</v>
-      </c>
-      <c r="Q1" s="1" t="s">
-        <v>621</v>
-      </c>
-      <c r="R1" s="1" t="s">
-        <v>622</v>
-      </c>
-      <c r="S1" s="1" t="s">
-        <v>623</v>
       </c>
       <c r="T1" s="1" t="s">
         <v>488</v>
       </c>
       <c r="U1" s="1" t="s">
-        <v>624</v>
+        <v>620</v>
       </c>
       <c r="V1" s="1" t="s">
         <v>223</v>
@@ -7774,10 +7781,10 @@
         <v>31</v>
       </c>
       <c r="AA1" s="56" t="s">
-        <v>625</v>
-      </c>
-    </row>
-    <row r="2" spans="1:27" ht="185.25" x14ac:dyDescent="0.45">
+        <v>621</v>
+      </c>
+    </row>
+    <row r="2" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B2" s="2" t="s">
         <v>379</v>
       </c>
@@ -7788,44 +7795,44 @@
         <v>396</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="I2" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J2" s="2" t="s">
-        <v>596</v>
+        <v>592</v>
       </c>
       <c r="K2" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L2" s="2" t="s">
-        <v>597</v>
+        <v>593</v>
       </c>
       <c r="M2" s="2">
         <v>1</v>
       </c>
       <c r="O2" s="82" t="s">
-        <v>722</v>
+        <v>718</v>
       </c>
       <c r="P2" s="82" t="s">
-        <v>599</v>
+        <v>595</v>
       </c>
       <c r="Q2" s="82" t="s">
-        <v>601</v>
+        <v>597</v>
       </c>
       <c r="R2" s="82" t="s">
         <v>481</v>
       </c>
       <c r="S2" s="2" t="s">
-        <v>602</v>
+        <v>598</v>
       </c>
       <c r="U2" s="2"/>
       <c r="AA2" s="82" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="3" spans="1:27" ht="185.25" x14ac:dyDescent="0.45">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="3" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B3" s="2" t="s">
         <v>379</v>
       </c>
@@ -7836,45 +7843,45 @@
         <v>396</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>694</v>
+        <v>690</v>
       </c>
       <c r="I3" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J3" s="2" t="s">
         <v>467</v>
       </c>
       <c r="K3" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L3" s="2" t="s">
-        <v>531</v>
+        <v>527</v>
       </c>
       <c r="M3" s="2">
         <v>1</v>
       </c>
       <c r="N3" s="82"/>
       <c r="O3" s="82" t="s">
-        <v>723</v>
+        <v>719</v>
       </c>
       <c r="P3" s="82" t="s">
+        <v>596</v>
+      </c>
+      <c r="Q3" s="82" t="s">
         <v>600</v>
       </c>
-      <c r="Q3" s="82" t="s">
-        <v>604</v>
-      </c>
       <c r="R3" s="82" t="s">
-        <v>598</v>
+        <v>594</v>
       </c>
       <c r="S3" s="2" t="s">
-        <v>603</v>
+        <v>599</v>
       </c>
       <c r="U3" s="2"/>
       <c r="AA3" s="82" t="s">
-        <v>589</v>
-      </c>
-    </row>
-    <row r="4" spans="1:27" ht="313.5" x14ac:dyDescent="0.45">
+        <v>585</v>
+      </c>
+    </row>
+    <row r="4" spans="1:27" ht="171" x14ac:dyDescent="0.45">
       <c r="B4" s="2" t="s">
         <v>381</v>
       </c>
@@ -7885,41 +7892,41 @@
         <v>398</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>712</v>
+        <v>708</v>
       </c>
       <c r="I4" s="2" t="s">
-        <v>536</v>
+        <v>532</v>
       </c>
       <c r="J4" s="2" t="s">
-        <v>534</v>
+        <v>530</v>
       </c>
       <c r="K4" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L4" s="2" t="s">
+        <v>533</v>
+      </c>
+      <c r="M4" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="O4" s="2" t="s">
         <v>537</v>
       </c>
-      <c r="M4" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="O4" s="2" t="s">
-        <v>541</v>
-      </c>
       <c r="P4" s="2" t="s">
-        <v>542</v>
+        <v>538</v>
       </c>
       <c r="Q4" s="2" t="s">
-        <v>539</v>
+        <v>535</v>
       </c>
       <c r="R4" s="2" t="s">
         <v>481</v>
       </c>
       <c r="S4" s="2" t="s">
-        <v>537</v>
+        <v>533</v>
       </c>
       <c r="U4" s="2"/>
     </row>
-    <row r="5" spans="1:27" ht="313.5" x14ac:dyDescent="0.45">
+    <row r="5" spans="1:27" ht="171" x14ac:dyDescent="0.45">
       <c r="B5" s="2" t="s">
         <v>381</v>
       </c>
@@ -7930,37 +7937,37 @@
         <v>398</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>713</v>
+        <v>709</v>
       </c>
       <c r="I5" s="2" t="s">
+        <v>532</v>
+      </c>
+      <c r="J5" s="2" t="s">
+        <v>531</v>
+      </c>
+      <c r="K5" s="2" t="s">
+        <v>546</v>
+      </c>
+      <c r="L5" s="2" t="s">
+        <v>534</v>
+      </c>
+      <c r="M5" s="2" t="s">
+        <v>529</v>
+      </c>
+      <c r="O5" s="82" t="s">
+        <v>754</v>
+      </c>
+      <c r="P5" s="82" t="s">
+        <v>721</v>
+      </c>
+      <c r="Q5" s="82" t="s">
+        <v>755</v>
+      </c>
+      <c r="R5" s="82" t="s">
+        <v>756</v>
+      </c>
+      <c r="S5" s="2" t="s">
         <v>536</v>
-      </c>
-      <c r="J5" s="2" t="s">
-        <v>535</v>
-      </c>
-      <c r="K5" s="2" t="s">
-        <v>550</v>
-      </c>
-      <c r="L5" s="2" t="s">
-        <v>538</v>
-      </c>
-      <c r="M5" s="2" t="s">
-        <v>533</v>
-      </c>
-      <c r="O5" s="82" t="s">
-        <v>725</v>
-      </c>
-      <c r="P5" s="82" t="s">
-        <v>726</v>
-      </c>
-      <c r="Q5" s="82" t="s">
-        <v>727</v>
-      </c>
-      <c r="R5" s="82" t="s">
-        <v>481</v>
-      </c>
-      <c r="S5" s="2" t="s">
-        <v>540</v>
       </c>
       <c r="U5" s="2"/>
     </row>
@@ -7975,7 +7982,7 @@
         <v>438</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>691</v>
+        <v>687</v>
       </c>
       <c r="I6" s="2" t="s">
         <v>505</v>
@@ -7984,7 +7991,7 @@
         <v>458</v>
       </c>
       <c r="K6" s="2" t="s">
-        <v>569</v>
+        <v>565</v>
       </c>
       <c r="L6" s="2" t="s">
         <v>506</v>
@@ -7993,23 +8000,23 @@
         <v>479</v>
       </c>
       <c r="O6" s="2" t="s">
-        <v>507</v>
+        <v>758</v>
       </c>
       <c r="P6" s="2" t="s">
         <v>495</v>
       </c>
       <c r="Q6" s="2" t="s">
-        <v>508</v>
+        <v>759</v>
       </c>
       <c r="R6" s="2" t="s">
-        <v>481</v>
+        <v>761</v>
       </c>
       <c r="S6" s="2" t="s">
         <v>506</v>
       </c>
       <c r="U6" s="2"/>
       <c r="AA6" s="82" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="7" spans="1:27" ht="71.25" x14ac:dyDescent="0.45">
@@ -8023,7 +8030,7 @@
         <v>437</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>692</v>
+        <v>688</v>
       </c>
       <c r="I7" s="2" t="s">
         <v>505</v>
@@ -8032,35 +8039,35 @@
         <v>459</v>
       </c>
       <c r="K7" s="2" t="s">
-        <v>570</v>
+        <v>566</v>
       </c>
       <c r="L7" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="M7" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O7" s="2" t="s">
-        <v>511</v>
+        <v>757</v>
       </c>
       <c r="P7" s="2" t="s">
         <v>495</v>
       </c>
       <c r="Q7" s="2" t="s">
-        <v>509</v>
+        <v>760</v>
       </c>
       <c r="R7" s="2" t="s">
-        <v>481</v>
+        <v>762</v>
       </c>
       <c r="S7" s="2" t="s">
-        <v>510</v>
+        <v>507</v>
       </c>
       <c r="U7" s="2"/>
       <c r="AA7" s="82" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="8" spans="1:27" ht="114" x14ac:dyDescent="0.45">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="8" spans="1:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B8" s="2" t="s">
         <v>445</v>
       </c>
@@ -8071,41 +8078,41 @@
         <v>393</v>
       </c>
       <c r="E8" s="83" t="s">
-        <v>693</v>
+        <v>689</v>
       </c>
       <c r="I8" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="J8" s="2" t="s">
         <v>455</v>
       </c>
       <c r="K8" s="2" t="s">
-        <v>568</v>
+        <v>564</v>
       </c>
       <c r="L8" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="M8" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O8" s="2" t="s">
-        <v>516</v>
+        <v>512</v>
       </c>
       <c r="P8" s="2" t="s">
-        <v>582</v>
+        <v>578</v>
       </c>
       <c r="Q8" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="R8" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="S8" s="2" t="s">
-        <v>513</v>
+        <v>509</v>
       </c>
       <c r="U8" s="2"/>
       <c r="AA8" s="82" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="9" spans="1:27" ht="114" x14ac:dyDescent="0.45">
@@ -8119,7 +8126,7 @@
         <v>435</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>709</v>
+        <v>705</v>
       </c>
       <c r="I9" s="2" t="s">
         <v>492</v>
@@ -8128,7 +8135,7 @@
         <v>457</v>
       </c>
       <c r="K9" s="2" t="s">
-        <v>566</v>
+        <v>562</v>
       </c>
       <c r="L9" s="2" t="s">
         <v>491</v>
@@ -8140,7 +8147,7 @@
         <v>493</v>
       </c>
       <c r="P9" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="Q9" s="2" t="s">
         <v>498</v>
@@ -8149,11 +8156,11 @@
         <v>481</v>
       </c>
       <c r="S9" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="U9" s="2"/>
       <c r="AA9" s="82" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="114" x14ac:dyDescent="0.45">
@@ -8167,7 +8174,7 @@
         <v>439</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>710</v>
+        <v>706</v>
       </c>
       <c r="I10" s="2" t="s">
         <v>492</v>
@@ -8176,7 +8183,7 @@
         <v>454</v>
       </c>
       <c r="K10" s="2" t="s">
-        <v>567</v>
+        <v>563</v>
       </c>
       <c r="L10" s="2" t="s">
         <v>500</v>
@@ -8197,11 +8204,11 @@
         <v>504</v>
       </c>
       <c r="S10" s="2" t="s">
-        <v>579</v>
+        <v>575</v>
       </c>
       <c r="U10" s="2"/>
       <c r="AA10" s="82" t="s">
-        <v>590</v>
+        <v>586</v>
       </c>
     </row>
     <row r="11" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
@@ -8215,7 +8222,7 @@
         <v>436</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>741</v>
+        <v>735</v>
       </c>
       <c r="I11" s="2" t="s">
         <v>476</v>
@@ -8233,26 +8240,26 @@
         <v>479</v>
       </c>
       <c r="O11" s="2" t="s">
-        <v>728</v>
+        <v>722</v>
       </c>
       <c r="P11" s="2" t="s">
         <v>494</v>
       </c>
       <c r="Q11" s="2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="R11" s="2" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="S11" s="2" t="s">
         <v>499</v>
       </c>
       <c r="U11" s="2"/>
       <c r="AA11" s="82" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="12" spans="1:27" ht="171" x14ac:dyDescent="0.45">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="12" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B12" s="2" t="s">
         <v>446</v>
       </c>
@@ -8266,41 +8273,41 @@
         <v>999999999</v>
       </c>
       <c r="I12" s="2" t="s">
-        <v>512</v>
+        <v>508</v>
       </c>
       <c r="J12" s="2" t="s">
         <v>456</v>
       </c>
       <c r="K12" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L12" s="2" t="s">
-        <v>517</v>
+        <v>513</v>
       </c>
       <c r="M12" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O12" s="2" t="s">
-        <v>519</v>
+        <v>515</v>
       </c>
       <c r="P12" s="2" t="s">
-        <v>581</v>
+        <v>577</v>
       </c>
       <c r="Q12" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="R12" s="2" t="s">
         <v>489</v>
       </c>
       <c r="S12" s="2" t="s">
-        <v>580</v>
+        <v>576</v>
       </c>
       <c r="U12" s="2"/>
       <c r="AA12" s="82" t="s">
-        <v>590</v>
-      </c>
-    </row>
-    <row r="13" spans="1:27" ht="114" x14ac:dyDescent="0.45">
+        <v>586</v>
+      </c>
+    </row>
+    <row r="13" spans="1:27" ht="57" x14ac:dyDescent="0.45">
       <c r="B13" s="2" t="s">
         <v>390</v>
       </c>
@@ -8311,41 +8318,41 @@
         <v>419</v>
       </c>
       <c r="E13" s="85" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="I13" s="2" t="s">
-        <v>520</v>
+        <v>516</v>
       </c>
       <c r="J13" s="2" t="s">
-        <v>521</v>
+        <v>517</v>
       </c>
       <c r="K13" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="L13" s="2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="M13" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O13" s="2" t="s">
-        <v>729</v>
+        <v>723</v>
       </c>
       <c r="P13" s="2" t="s">
-        <v>627</v>
+        <v>623</v>
       </c>
       <c r="Q13" s="2" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="R13" s="2" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="S13" s="2" t="s">
-        <v>557</v>
+        <v>553</v>
       </c>
       <c r="U13" s="2"/>
       <c r="AA13" s="82" t="s">
-        <v>592</v>
+        <v>588</v>
       </c>
     </row>
     <row r="14" spans="1:27" ht="114" x14ac:dyDescent="0.45">
@@ -8359,7 +8366,7 @@
         <v>421</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>718</v>
+        <v>714</v>
       </c>
       <c r="I14" s="2" t="s">
         <v>492</v>
@@ -8377,10 +8384,10 @@
         <v>479</v>
       </c>
       <c r="O14" s="2" t="s">
-        <v>670</v>
+        <v>666</v>
       </c>
       <c r="P14" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="Q14" s="2" t="s">
         <v>498</v>
@@ -8389,11 +8396,11 @@
         <v>481</v>
       </c>
       <c r="S14" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="U14" s="2"/>
       <c r="AA14" s="82" t="s">
-        <v>593</v>
+        <v>589</v>
       </c>
     </row>
     <row r="15" spans="1:27" ht="85.5" x14ac:dyDescent="0.45">
@@ -8407,7 +8414,7 @@
         <v>420</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>742</v>
+        <v>736</v>
       </c>
       <c r="I15" s="2" t="s">
         <v>476</v>
@@ -8425,23 +8432,23 @@
         <v>1</v>
       </c>
       <c r="O15" s="2" t="s">
-        <v>730</v>
+        <v>724</v>
       </c>
       <c r="P15" s="2" t="s">
         <v>494</v>
       </c>
       <c r="Q15" s="2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="R15" s="2" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="S15" s="2" t="s">
         <v>499</v>
       </c>
       <c r="U15" s="2"/>
     </row>
-    <row r="16" spans="1:27" ht="171" x14ac:dyDescent="0.45">
+    <row r="16" spans="1:27" ht="156.75" x14ac:dyDescent="0.45">
       <c r="B16" s="2" t="s">
         <v>374</v>
       </c>
@@ -8461,7 +8468,7 @@
         <v>450</v>
       </c>
       <c r="K16" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L16" s="2" t="s">
         <v>480</v>
@@ -8470,10 +8477,10 @@
         <v>479</v>
       </c>
       <c r="O16" s="82" t="s">
-        <v>719</v>
+        <v>715</v>
       </c>
       <c r="P16" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="Q16" s="2" t="s">
         <v>482</v>
@@ -8482,11 +8489,11 @@
         <v>481</v>
       </c>
       <c r="S16" s="2" t="s">
-        <v>577</v>
+        <v>573</v>
       </c>
       <c r="U16" s="2"/>
     </row>
-    <row r="17" spans="2:27" ht="142.5" x14ac:dyDescent="0.45">
+    <row r="17" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B17" s="2" t="s">
         <v>373</v>
       </c>
@@ -8497,7 +8504,7 @@
         <v>448</v>
       </c>
       <c r="E17" s="2" t="s">
-        <v>688</v>
+        <v>684</v>
       </c>
       <c r="I17" s="2" t="s">
         <v>475</v>
@@ -8506,7 +8513,7 @@
         <v>474</v>
       </c>
       <c r="K17" s="2" t="s">
-        <v>565</v>
+        <v>561</v>
       </c>
       <c r="L17" s="2" t="s">
         <v>478</v>
@@ -8515,23 +8522,23 @@
         <v>479</v>
       </c>
       <c r="O17" s="82" t="s">
-        <v>731</v>
+        <v>725</v>
       </c>
       <c r="P17" s="2" t="s">
-        <v>585</v>
+        <v>581</v>
       </c>
       <c r="Q17" s="2" t="s">
-        <v>732</v>
+        <v>726</v>
       </c>
       <c r="R17" s="2" t="s">
         <v>481</v>
       </c>
       <c r="S17" s="2" t="s">
-        <v>576</v>
+        <v>572</v>
       </c>
       <c r="U17" s="2"/>
     </row>
-    <row r="18" spans="2:27" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="18" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B18" s="2" t="s">
         <v>375</v>
       </c>
@@ -8542,7 +8549,7 @@
         <v>429</v>
       </c>
       <c r="E18" s="2" t="s">
-        <v>689</v>
+        <v>685</v>
       </c>
       <c r="I18" s="2" t="s">
         <v>475</v>
@@ -8551,7 +8558,7 @@
         <v>449</v>
       </c>
       <c r="K18" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L18" s="2" t="s">
         <v>483</v>
@@ -8560,7 +8567,7 @@
         <v>479</v>
       </c>
       <c r="O18" s="2" t="s">
-        <v>720</v>
+        <v>716</v>
       </c>
       <c r="P18" s="2" t="s">
         <v>497</v>
@@ -8572,11 +8579,11 @@
         <v>481</v>
       </c>
       <c r="S18" s="2" t="s">
-        <v>575</v>
+        <v>571</v>
       </c>
       <c r="U18" s="2"/>
       <c r="AA18" s="82" t="s">
-        <v>594</v>
+        <v>590</v>
       </c>
     </row>
     <row r="19" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
@@ -8590,37 +8597,37 @@
         <v>403</v>
       </c>
       <c r="E19" s="85" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="I19" s="2" t="s">
-        <v>677</v>
+        <v>673</v>
       </c>
       <c r="J19" s="2" t="s">
-        <v>678</v>
+        <v>674</v>
       </c>
       <c r="K19" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="L19" s="2" t="s">
-        <v>679</v>
+        <v>675</v>
       </c>
       <c r="M19" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O19" s="2" t="s">
-        <v>724</v>
+        <v>720</v>
       </c>
       <c r="P19" s="2" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="Q19" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="R19" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="S19" s="2" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="U19" s="2"/>
     </row>
@@ -8635,7 +8642,7 @@
         <v>418</v>
       </c>
       <c r="E20" s="2" t="s">
-        <v>717</v>
+        <v>713</v>
       </c>
       <c r="I20" s="2" t="s">
         <v>492</v>
@@ -8653,10 +8660,10 @@
         <v>479</v>
       </c>
       <c r="O20" s="2" t="s">
-        <v>674</v>
+        <v>670</v>
       </c>
       <c r="P20" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="Q20" s="2" t="s">
         <v>498</v>
@@ -8665,7 +8672,7 @@
         <v>481</v>
       </c>
       <c r="S20" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="U20" s="2"/>
     </row>
@@ -8680,7 +8687,7 @@
         <v>416</v>
       </c>
       <c r="E21" s="85" t="s">
-        <v>716</v>
+        <v>712</v>
       </c>
       <c r="I21" s="2" t="s">
         <v>476</v>
@@ -8698,16 +8705,16 @@
         <v>1</v>
       </c>
       <c r="O21" s="2" t="s">
-        <v>673</v>
+        <v>669</v>
       </c>
       <c r="P21" s="2" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="Q21" s="2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="R21" s="2" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="S21" s="2" t="s">
         <v>499</v>
@@ -8725,7 +8732,7 @@
         <v>417</v>
       </c>
       <c r="E22" s="2" t="s">
-        <v>708</v>
+        <v>704</v>
       </c>
       <c r="I22" s="2" t="s">
         <v>492</v>
@@ -8743,10 +8750,10 @@
         <v>479</v>
       </c>
       <c r="O22" s="2" t="s">
-        <v>672</v>
+        <v>668</v>
       </c>
       <c r="P22" s="2" t="s">
-        <v>583</v>
+        <v>579</v>
       </c>
       <c r="Q22" s="2" t="s">
         <v>498</v>
@@ -8755,11 +8762,11 @@
         <v>481</v>
       </c>
       <c r="S22" s="2" t="s">
-        <v>584</v>
+        <v>580</v>
       </c>
       <c r="U22" s="2"/>
       <c r="AA22" s="82" t="s">
-        <v>595</v>
+        <v>591</v>
       </c>
     </row>
     <row r="23" spans="2:27" ht="114" x14ac:dyDescent="0.45">
@@ -8773,7 +8780,7 @@
         <v>414</v>
       </c>
       <c r="E23" s="85" t="s">
-        <v>707</v>
+        <v>703</v>
       </c>
       <c r="I23" s="2" t="s">
         <v>476</v>
@@ -8791,23 +8798,23 @@
         <v>1</v>
       </c>
       <c r="O23" s="2" t="s">
-        <v>671</v>
+        <v>667</v>
       </c>
       <c r="P23" s="2" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="Q23" s="2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="R23" s="2" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="S23" s="2" t="s">
         <v>499</v>
       </c>
       <c r="U23" s="2"/>
     </row>
-    <row r="24" spans="2:27" ht="185.25" x14ac:dyDescent="0.45">
+    <row r="24" spans="2:27" ht="128.25" x14ac:dyDescent="0.45">
       <c r="B24" s="2" t="s">
         <v>376</v>
       </c>
@@ -8818,7 +8825,7 @@
         <v>430</v>
       </c>
       <c r="E24" s="2" t="s">
-        <v>690</v>
+        <v>686</v>
       </c>
       <c r="I24" s="2" t="s">
         <v>477</v>
@@ -8827,7 +8834,7 @@
         <v>451</v>
       </c>
       <c r="K24" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L24" s="2" t="s">
         <v>487</v>
@@ -8836,7 +8843,7 @@
         <v>479</v>
       </c>
       <c r="O24" s="2" t="s">
-        <v>733</v>
+        <v>727</v>
       </c>
       <c r="P24" s="2" t="s">
         <v>496</v>
@@ -8848,11 +8855,11 @@
         <v>489</v>
       </c>
       <c r="S24" s="2" t="s">
-        <v>578</v>
+        <v>574</v>
       </c>
       <c r="U24" s="2"/>
       <c r="AA24" s="82" t="s">
-        <v>591</v>
+        <v>587</v>
       </c>
     </row>
     <row r="25" spans="2:27" ht="114" x14ac:dyDescent="0.45">
@@ -8866,7 +8873,7 @@
         <v>413</v>
       </c>
       <c r="E25" s="85" t="s">
-        <v>706</v>
+        <v>702</v>
       </c>
       <c r="I25" s="2" t="s">
         <v>94</v>
@@ -8875,28 +8882,28 @@
         <v>453</v>
       </c>
       <c r="K25" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L25" s="2" t="s">
-        <v>664</v>
+        <v>660</v>
       </c>
       <c r="M25" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O25" s="2" t="s">
-        <v>667</v>
+        <v>663</v>
       </c>
       <c r="P25" s="2" t="s">
-        <v>668</v>
+        <v>664</v>
       </c>
       <c r="Q25" s="2" t="s">
+        <v>661</v>
+      </c>
+      <c r="R25" s="2" t="s">
+        <v>662</v>
+      </c>
+      <c r="S25" s="2" t="s">
         <v>665</v>
-      </c>
-      <c r="R25" s="2" t="s">
-        <v>666</v>
-      </c>
-      <c r="S25" s="2" t="s">
-        <v>669</v>
       </c>
       <c r="U25" s="2"/>
     </row>
@@ -8911,7 +8918,7 @@
         <v>415</v>
       </c>
       <c r="E26" s="85" t="s">
-        <v>715</v>
+        <v>711</v>
       </c>
       <c r="I26" s="2" t="s">
         <v>476</v>
@@ -8929,19 +8936,19 @@
         <v>1</v>
       </c>
       <c r="O26" s="82" t="s">
-        <v>675</v>
+        <v>671</v>
       </c>
       <c r="P26" s="2" t="s">
-        <v>676</v>
+        <v>672</v>
       </c>
       <c r="Q26" s="2" t="s">
-        <v>665</v>
+        <v>661</v>
       </c>
       <c r="R26" s="2" t="s">
-        <v>666</v>
+        <v>662</v>
       </c>
       <c r="S26" s="82" t="s">
-        <v>685</v>
+        <v>681</v>
       </c>
       <c r="U26" s="2"/>
     </row>
@@ -8956,41 +8963,41 @@
         <v>410</v>
       </c>
       <c r="E27" s="2" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="I27" s="2" t="s">
         <v>471</v>
       </c>
       <c r="J27" s="2" t="s">
-        <v>644</v>
+        <v>640</v>
       </c>
       <c r="K27" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L27" s="2" t="s">
-        <v>645</v>
+        <v>641</v>
       </c>
       <c r="M27" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O27" s="2" t="s">
-        <v>647</v>
+        <v>643</v>
       </c>
       <c r="P27" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="Q27" s="2" t="s">
-        <v>646</v>
+        <v>642</v>
       </c>
       <c r="R27" s="2" t="s">
         <v>481</v>
       </c>
       <c r="S27" s="2" t="s">
-        <v>648</v>
+        <v>644</v>
       </c>
       <c r="U27" s="2"/>
     </row>
-    <row r="28" spans="2:27" ht="171" x14ac:dyDescent="0.45">
+    <row r="28" spans="2:27" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B28" s="2" t="s">
         <v>378</v>
       </c>
@@ -9004,35 +9011,35 @@
         <v>1</v>
       </c>
       <c r="I28" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J28" s="2" t="s">
         <v>466</v>
       </c>
       <c r="K28" s="2" t="s">
-        <v>546</v>
+        <v>542</v>
       </c>
       <c r="L28" s="2" t="s">
-        <v>527</v>
+        <v>523</v>
       </c>
       <c r="M28" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O28" s="2" t="s">
-        <v>735</v>
+        <v>729</v>
       </c>
       <c r="Q28" s="2" t="s">
-        <v>528</v>
+        <v>524</v>
       </c>
       <c r="R28" s="2" t="s">
-        <v>529</v>
+        <v>525</v>
       </c>
       <c r="S28" s="2" t="s">
-        <v>588</v>
+        <v>584</v>
       </c>
       <c r="U28" s="2"/>
     </row>
-    <row r="29" spans="2:27" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="29" spans="2:27" ht="99.75" x14ac:dyDescent="0.45">
       <c r="B29" s="2" t="s">
         <v>389</v>
       </c>
@@ -9049,35 +9056,35 @@
         <v>471</v>
       </c>
       <c r="J29" s="2" t="s">
-        <v>523</v>
+        <v>519</v>
       </c>
       <c r="K29" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L29" s="2" t="s">
-        <v>522</v>
+        <v>518</v>
       </c>
       <c r="M29" s="2">
         <v>1</v>
       </c>
       <c r="O29" s="2" t="s">
-        <v>734</v>
+        <v>728</v>
       </c>
       <c r="P29" s="2" t="s">
-        <v>574</v>
+        <v>570</v>
       </c>
       <c r="Q29" s="2" t="s">
-        <v>524</v>
+        <v>520</v>
       </c>
       <c r="R29" s="2" t="s">
         <v>481</v>
       </c>
       <c r="S29" s="2" t="s">
-        <v>573</v>
+        <v>569</v>
       </c>
       <c r="U29" s="2"/>
     </row>
-    <row r="30" spans="2:27" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="30" spans="2:27" ht="213.75" x14ac:dyDescent="0.45">
       <c r="B30" s="2" t="s">
         <v>380</v>
       </c>
@@ -9091,39 +9098,39 @@
         <v>0.6020833333333333</v>
       </c>
       <c r="I30" s="2" t="s">
-        <v>530</v>
+        <v>526</v>
       </c>
       <c r="J30" s="2" t="s">
         <v>468</v>
       </c>
       <c r="K30" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L30" s="2" t="s">
-        <v>532</v>
+        <v>528</v>
       </c>
       <c r="M30" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="N30" s="82"/>
       <c r="O30" s="82" t="s">
-        <v>737</v>
+        <v>731</v>
       </c>
       <c r="P30" s="82" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="Q30" s="82" t="s">
-        <v>605</v>
+        <v>601</v>
       </c>
       <c r="R30" s="82" t="s">
-        <v>606</v>
+        <v>602</v>
       </c>
       <c r="S30" s="2" t="s">
-        <v>607</v>
+        <v>603</v>
       </c>
       <c r="U30" s="2"/>
     </row>
-    <row r="31" spans="2:27" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="31" spans="2:27" ht="299.25" x14ac:dyDescent="0.45">
       <c r="B31" s="2" t="s">
         <v>377</v>
       </c>
@@ -9134,41 +9141,41 @@
         <v>394</v>
       </c>
       <c r="E31" s="2" t="s">
-        <v>711</v>
+        <v>707</v>
       </c>
       <c r="I31" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J31" s="2" t="s">
         <v>465</v>
       </c>
       <c r="K31" s="2" t="s">
-        <v>571</v>
+        <v>567</v>
       </c>
       <c r="L31" s="2" t="s">
-        <v>526</v>
+        <v>522</v>
       </c>
       <c r="M31" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O31" s="2" t="s">
-        <v>736</v>
+        <v>730</v>
       </c>
       <c r="P31" s="2" t="s">
-        <v>586</v>
+        <v>582</v>
       </c>
       <c r="Q31" s="2" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="R31" s="2" t="s">
         <v>489</v>
       </c>
       <c r="S31" s="2" t="s">
-        <v>587</v>
+        <v>583</v>
       </c>
       <c r="U31" s="2"/>
     </row>
-    <row r="32" spans="2:27" ht="156.75" x14ac:dyDescent="0.45">
+    <row r="32" spans="2:27" ht="85.5" x14ac:dyDescent="0.45">
       <c r="B32" s="2" t="s">
         <v>383</v>
       </c>
@@ -9179,41 +9186,41 @@
         <v>402</v>
       </c>
       <c r="E32" s="85" t="s">
-        <v>695</v>
+        <v>691</v>
       </c>
       <c r="I32" s="2" t="s">
+        <v>548</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>550</v>
+      </c>
+      <c r="K32" s="2" t="s">
+        <v>551</v>
+      </c>
+      <c r="L32" s="2" t="s">
         <v>552</v>
-      </c>
-      <c r="J32" s="2" t="s">
-        <v>554</v>
-      </c>
-      <c r="K32" s="2" t="s">
-        <v>555</v>
-      </c>
-      <c r="L32" s="2" t="s">
-        <v>556</v>
       </c>
       <c r="M32" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O32" s="82" t="s">
-        <v>721</v>
+        <v>717</v>
       </c>
       <c r="P32" s="82" t="s">
-        <v>626</v>
+        <v>622</v>
       </c>
       <c r="Q32" s="2" t="s">
-        <v>514</v>
+        <v>510</v>
       </c>
       <c r="R32" s="2" t="s">
-        <v>515</v>
+        <v>511</v>
       </c>
       <c r="S32" s="82" t="s">
-        <v>556</v>
+        <v>552</v>
       </c>
       <c r="U32" s="2"/>
     </row>
-    <row r="33" spans="2:21" ht="256.5" x14ac:dyDescent="0.45">
+    <row r="33" spans="2:21" ht="114" x14ac:dyDescent="0.45">
       <c r="B33" s="2" t="s">
         <v>362</v>
       </c>
@@ -9224,16 +9231,16 @@
         <v>412</v>
       </c>
       <c r="E33" s="2" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="I33" s="2" t="s">
-        <v>654</v>
+        <v>650</v>
       </c>
       <c r="J33" s="2" t="s">
         <v>473</v>
       </c>
       <c r="K33" s="2" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="L33" s="82" t="s">
         <v>412</v>
@@ -9242,23 +9249,23 @@
         <v>479</v>
       </c>
       <c r="O33" s="2" t="s">
-        <v>653</v>
+        <v>649</v>
       </c>
       <c r="P33" s="2" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="Q33" s="2" t="s">
-        <v>651</v>
+        <v>647</v>
       </c>
       <c r="R33" s="2" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="S33" s="2" t="s">
-        <v>652</v>
+        <v>648</v>
       </c>
       <c r="U33" s="2"/>
     </row>
-    <row r="34" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="34" spans="2:21" ht="213.75" x14ac:dyDescent="0.45">
       <c r="B34" s="2" t="s">
         <v>363</v>
       </c>
@@ -9269,41 +9276,41 @@
         <v>432</v>
       </c>
       <c r="E34" s="2" t="s">
-        <v>703</v>
+        <v>699</v>
       </c>
       <c r="I34" s="2" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="J34" s="2" t="s">
-        <v>657</v>
+        <v>653</v>
       </c>
       <c r="K34" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L34" s="2" t="s">
-        <v>658</v>
+        <v>654</v>
       </c>
       <c r="M34" s="2">
         <v>1</v>
       </c>
       <c r="O34" s="82" t="s">
-        <v>659</v>
+        <v>655</v>
       </c>
       <c r="P34" s="82" t="s">
-        <v>613</v>
+        <v>609</v>
       </c>
       <c r="Q34" s="82" t="s">
-        <v>660</v>
+        <v>656</v>
       </c>
       <c r="R34" s="82" t="s">
         <v>481</v>
       </c>
       <c r="S34" s="82" t="s">
-        <v>661</v>
+        <v>657</v>
       </c>
       <c r="U34" s="2"/>
     </row>
-    <row r="35" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+    <row r="35" spans="2:21" ht="228" x14ac:dyDescent="0.45">
       <c r="B35" s="2" t="s">
         <v>382</v>
       </c>
@@ -9314,37 +9321,37 @@
         <v>399</v>
       </c>
       <c r="E35" s="2" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="I35" s="2" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J35" s="2" t="s">
-        <v>655</v>
+        <v>651</v>
       </c>
       <c r="K35" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L35" s="2" t="s">
-        <v>656</v>
+        <v>652</v>
       </c>
       <c r="M35" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O35" s="2" t="s">
-        <v>615</v>
+        <v>611</v>
       </c>
       <c r="P35" s="2" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="Q35" s="2" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="R35" s="2" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="S35" s="2" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="U35" s="2"/>
     </row>
@@ -9356,44 +9363,44 @@
         <v>424</v>
       </c>
       <c r="D36" s="2" t="s">
-        <v>750</v>
+        <v>744</v>
       </c>
       <c r="E36" s="2" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="I36" s="2" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J36" s="2" t="s">
-        <v>752</v>
+        <v>746</v>
       </c>
       <c r="K36" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L36" s="2" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="M36" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O36" s="82" t="s">
-        <v>747</v>
+        <v>741</v>
       </c>
       <c r="P36" s="82" t="s">
-        <v>748</v>
+        <v>742</v>
       </c>
       <c r="Q36" s="82" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="R36" s="82" t="s">
-        <v>749</v>
+        <v>743</v>
       </c>
       <c r="S36" s="82" t="s">
-        <v>751</v>
+        <v>745</v>
       </c>
       <c r="U36" s="2"/>
     </row>
-    <row r="37" spans="2:21" ht="171" x14ac:dyDescent="0.45">
+    <row r="37" spans="2:21" ht="71.25" x14ac:dyDescent="0.45">
       <c r="B37" s="2" t="s">
         <v>372</v>
       </c>
@@ -9404,16 +9411,16 @@
         <v>404</v>
       </c>
       <c r="E37" s="85" t="s">
-        <v>696</v>
+        <v>692</v>
       </c>
       <c r="I37" s="2" t="s">
-        <v>553</v>
+        <v>549</v>
       </c>
       <c r="J37" s="2" t="s">
         <v>461</v>
       </c>
       <c r="K37" s="2" t="s">
-        <v>560</v>
+        <v>556</v>
       </c>
       <c r="L37" s="82" t="s">
         <v>404</v>
@@ -9422,19 +9429,19 @@
         <v>479</v>
       </c>
       <c r="O37" s="2" t="s">
-        <v>561</v>
+        <v>557</v>
       </c>
       <c r="P37" s="82" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="Q37" s="82" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="R37" s="82" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="S37" s="82" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="U37" s="2"/>
     </row>
@@ -9449,37 +9456,37 @@
         <v>400</v>
       </c>
       <c r="E38" s="2" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="I38" s="2" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="J38" s="2" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="K38" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L38" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="M38" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O38" s="82" t="s">
-        <v>618</v>
+        <v>614</v>
       </c>
       <c r="P38" s="82" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="Q38" s="82" t="s">
-        <v>614</v>
+        <v>610</v>
       </c>
       <c r="R38" s="82" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="S38" s="82" t="s">
-        <v>612</v>
+        <v>608</v>
       </c>
       <c r="U38" s="2"/>
     </row>
@@ -9494,37 +9501,37 @@
         <v>400</v>
       </c>
       <c r="E39" s="2" t="s">
-        <v>714</v>
+        <v>710</v>
       </c>
       <c r="I39" s="2" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="J39" s="2" t="s">
-        <v>549</v>
+        <v>545</v>
       </c>
       <c r="K39" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L39" s="2" t="s">
-        <v>551</v>
+        <v>547</v>
       </c>
       <c r="M39" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O39" s="82" t="s">
-        <v>743</v>
+        <v>737</v>
       </c>
       <c r="P39" s="82" t="s">
-        <v>547</v>
+        <v>543</v>
       </c>
       <c r="Q39" s="82" t="s">
-        <v>744</v>
+        <v>738</v>
       </c>
       <c r="R39" s="82" t="s">
-        <v>745</v>
+        <v>739</v>
       </c>
       <c r="S39" s="82" t="s">
-        <v>746</v>
+        <v>740</v>
       </c>
       <c r="U39" s="2"/>
     </row>
@@ -9539,37 +9546,37 @@
         <v>411</v>
       </c>
       <c r="E40" s="85" t="s">
-        <v>702</v>
+        <v>698</v>
       </c>
       <c r="I40" s="2" t="s">
-        <v>649</v>
+        <v>645</v>
       </c>
       <c r="J40" s="2" t="s">
         <v>472</v>
       </c>
       <c r="K40" s="2" t="s">
-        <v>650</v>
+        <v>646</v>
       </c>
       <c r="L40" s="82" t="s">
-        <v>686</v>
+        <v>682</v>
       </c>
       <c r="M40" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O40" s="82" t="s">
-        <v>617</v>
+        <v>613</v>
       </c>
       <c r="P40" s="82" t="s">
-        <v>616</v>
+        <v>612</v>
       </c>
       <c r="Q40" s="82" t="s">
-        <v>608</v>
+        <v>604</v>
       </c>
       <c r="R40" s="82" t="s">
-        <v>609</v>
+        <v>605</v>
       </c>
       <c r="S40" s="82" t="s">
-        <v>611</v>
+        <v>607</v>
       </c>
       <c r="U40" s="2"/>
     </row>
@@ -9584,37 +9591,37 @@
         <v>431</v>
       </c>
       <c r="E41" s="85" t="s">
-        <v>700</v>
+        <v>696</v>
       </c>
       <c r="I41" s="2" t="s">
         <v>470</v>
       </c>
       <c r="J41" s="2" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="K41" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L41" s="2" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="M41" s="2">
         <v>1</v>
       </c>
       <c r="O41" s="82" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="P41" s="82" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="Q41" s="82" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="R41" s="82" t="s">
         <v>489</v>
       </c>
       <c r="S41" s="82" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="U41" s="2"/>
     </row>
@@ -9629,37 +9636,37 @@
         <v>407</v>
       </c>
       <c r="E42" s="85" t="s">
-        <v>701</v>
+        <v>697</v>
       </c>
       <c r="I42" s="2" t="s">
         <v>470</v>
       </c>
       <c r="J42" s="2" t="s">
-        <v>639</v>
+        <v>635</v>
       </c>
       <c r="K42" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L42" s="2" t="s">
-        <v>638</v>
+        <v>634</v>
       </c>
       <c r="M42" s="2">
         <v>1</v>
       </c>
       <c r="O42" s="82" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="P42" s="82" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="Q42" s="82" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="R42" s="82" t="s">
         <v>489</v>
       </c>
       <c r="S42" s="82" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="U42" s="2"/>
     </row>
@@ -9674,37 +9681,37 @@
         <v>462</v>
       </c>
       <c r="E43" s="2" t="s">
-        <v>698</v>
+        <v>694</v>
       </c>
       <c r="I43" s="2" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="J43" s="2" t="s">
         <v>469</v>
       </c>
       <c r="K43" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L43" s="2" t="s">
-        <v>643</v>
+        <v>639</v>
       </c>
       <c r="M43" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="O43" s="82" t="s">
-        <v>738</v>
+        <v>732</v>
       </c>
       <c r="P43" s="82" t="s">
-        <v>640</v>
+        <v>636</v>
       </c>
       <c r="Q43" s="82" t="s">
-        <v>518</v>
+        <v>514</v>
       </c>
       <c r="R43" s="82" t="s">
         <v>489</v>
       </c>
       <c r="S43" s="82" t="s">
-        <v>642</v>
+        <v>638</v>
       </c>
       <c r="U43" s="2"/>
     </row>
@@ -9719,37 +9726,37 @@
         <v>406</v>
       </c>
       <c r="E44" s="2" t="s">
-        <v>699</v>
+        <v>695</v>
       </c>
       <c r="I44" s="2" t="s">
         <v>470</v>
       </c>
       <c r="J44" s="2" t="s">
-        <v>637</v>
+        <v>633</v>
       </c>
       <c r="K44" s="2" t="s">
-        <v>572</v>
+        <v>568</v>
       </c>
       <c r="L44" s="2" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="M44" s="2">
         <v>1</v>
       </c>
       <c r="O44" s="82" t="s">
-        <v>739</v>
+        <v>733</v>
       </c>
       <c r="P44" s="82" t="s">
-        <v>641</v>
+        <v>637</v>
       </c>
       <c r="Q44" s="82" t="s">
-        <v>635</v>
+        <v>631</v>
       </c>
       <c r="R44" s="82" t="s">
         <v>481</v>
       </c>
       <c r="S44" s="82" t="s">
-        <v>636</v>
+        <v>632</v>
       </c>
       <c r="U44" s="2"/>
     </row>
@@ -9764,7 +9771,7 @@
         <v>464</v>
       </c>
       <c r="E45" s="2" t="s">
-        <v>705</v>
+        <v>701</v>
       </c>
       <c r="I45" s="2" t="s">
         <v>460</v>
@@ -9773,22 +9780,22 @@
         <v>460</v>
       </c>
       <c r="K45" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L45" s="82" t="s">
         <v>464</v>
       </c>
       <c r="M45" s="2" t="s">
-        <v>533</v>
+        <v>529</v>
       </c>
       <c r="O45" s="2" t="s">
-        <v>740</v>
+        <v>734</v>
       </c>
       <c r="P45" s="2" t="s">
-        <v>662</v>
+        <v>658</v>
       </c>
       <c r="Q45" s="2" t="s">
-        <v>663</v>
+        <v>659</v>
       </c>
       <c r="R45" s="2" t="s">
         <v>481</v>
@@ -9809,16 +9816,16 @@
         <v>405</v>
       </c>
       <c r="E46" s="85" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="I46" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J46" s="2" t="s">
-        <v>564</v>
+        <v>560</v>
       </c>
       <c r="K46" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L46" s="82" t="s">
         <v>405</v>
@@ -9827,19 +9834,19 @@
         <v>479</v>
       </c>
       <c r="O46" s="82" t="s">
-        <v>631</v>
+        <v>627</v>
       </c>
       <c r="P46" s="82" t="s">
-        <v>634</v>
+        <v>630</v>
       </c>
       <c r="Q46" s="82" t="s">
-        <v>633</v>
+        <v>629</v>
       </c>
       <c r="R46" s="82" t="s">
-        <v>610</v>
+        <v>606</v>
       </c>
       <c r="S46" s="82" t="s">
-        <v>632</v>
+        <v>628</v>
       </c>
       <c r="U46" s="2"/>
     </row>
@@ -9854,16 +9861,16 @@
         <v>405</v>
       </c>
       <c r="E47" s="85" t="s">
-        <v>697</v>
+        <v>693</v>
       </c>
       <c r="I47" s="2" t="s">
-        <v>563</v>
+        <v>559</v>
       </c>
       <c r="J47" s="2" t="s">
-        <v>562</v>
+        <v>558</v>
       </c>
       <c r="K47" s="2" t="s">
-        <v>555</v>
+        <v>551</v>
       </c>
       <c r="L47" s="82" t="s">
         <v>405</v>
@@ -9872,19 +9879,19 @@
         <v>479</v>
       </c>
       <c r="O47" s="82" t="s">
-        <v>630</v>
+        <v>626</v>
       </c>
       <c r="P47" s="82" t="s">
-        <v>628</v>
+        <v>624</v>
       </c>
       <c r="Q47" s="82" t="s">
-        <v>558</v>
+        <v>554</v>
       </c>
       <c r="R47" s="82" t="s">
-        <v>559</v>
+        <v>555</v>
       </c>
       <c r="S47" s="82" t="s">
-        <v>629</v>
+        <v>625</v>
       </c>
       <c r="U47" s="2"/>
     </row>
@@ -9899,16 +9906,16 @@
         <v>463</v>
       </c>
       <c r="E48" s="2" t="s">
-        <v>704</v>
+        <v>700</v>
       </c>
       <c r="I48" s="82" t="s">
-        <v>548</v>
+        <v>544</v>
       </c>
       <c r="J48" s="82" t="s">
-        <v>684</v>
+        <v>680</v>
       </c>
       <c r="K48" s="82" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L48" s="82" t="s">
         <v>463</v>
@@ -9917,82 +9924,75 @@
         <v>479</v>
       </c>
       <c r="O48" s="82" t="s">
-        <v>680</v>
+        <v>676</v>
       </c>
       <c r="P48" s="82" t="s">
-        <v>681</v>
+        <v>677</v>
       </c>
       <c r="Q48" s="82" t="s">
-        <v>682</v>
+        <v>678</v>
       </c>
       <c r="R48" s="82" t="s">
         <v>481</v>
       </c>
       <c r="S48" s="82" t="s">
-        <v>683</v>
+        <v>679</v>
       </c>
       <c r="U48" s="2"/>
     </row>
-    <row r="49" spans="1:25" ht="409.5" x14ac:dyDescent="0.45">
-      <c r="A49" s="86"/>
-      <c r="B49" s="86" t="s">
-        <v>753</v>
-      </c>
-      <c r="C49" s="86" t="s">
-        <v>754</v>
+    <row r="49" spans="2:21" ht="409.5" x14ac:dyDescent="0.45">
+      <c r="B49" s="2" t="s">
+        <v>747</v>
+      </c>
+      <c r="C49" s="2" t="s">
+        <v>748</v>
       </c>
       <c r="D49" s="2" t="s">
-        <v>755</v>
-      </c>
-      <c r="E49" s="86">
+        <v>749</v>
+      </c>
+      <c r="E49" s="2">
         <v>1125</v>
       </c>
-      <c r="F49" s="86">
+      <c r="F49" s="2">
         <v>1125</v>
       </c>
-      <c r="G49" s="86"/>
-      <c r="H49" s="86"/>
       <c r="I49" s="2" t="s">
-        <v>525</v>
+        <v>521</v>
       </c>
       <c r="J49" s="2" t="s">
-        <v>753</v>
+        <v>747</v>
       </c>
       <c r="K49" s="2" t="s">
-        <v>550</v>
+        <v>546</v>
       </c>
       <c r="L49" s="2" t="s">
-        <v>756</v>
+        <v>750</v>
       </c>
       <c r="M49" s="2">
         <v>1</v>
       </c>
-      <c r="N49" s="86" t="s">
+      <c r="N49" s="2" t="s">
         <v>479</v>
       </c>
       <c r="O49" s="2" t="s">
-        <v>757</v>
-      </c>
-      <c r="P49" s="86" t="s">
-        <v>758</v>
-      </c>
-      <c r="Q49" s="86" t="s">
-        <v>759</v>
-      </c>
-      <c r="R49" s="86" t="s">
+        <v>751</v>
+      </c>
+      <c r="P49" s="2" t="s">
+        <v>752</v>
+      </c>
+      <c r="Q49" s="2" t="s">
+        <v>753</v>
+      </c>
+      <c r="R49" s="2" t="s">
         <v>489</v>
       </c>
-      <c r="S49" s="86" t="s">
-        <v>756</v>
+      <c r="S49" s="2" t="s">
+        <v>750</v>
       </c>
       <c r="T49" s="2" t="s">
-        <v>756</v>
-      </c>
-      <c r="U49" s="86"/>
-      <c r="V49" s="86"/>
-      <c r="W49" s="86"/>
-      <c r="X49" s="86"/>
-      <c r="Y49" s="86"/>
+        <v>750</v>
+      </c>
+      <c r="U49" s="2"/>
     </row>
   </sheetData>
   <phoneticPr fontId="19" type="noConversion"/>

</xml_diff>